<commit_message>
Added connector pinout drawings for Dyno Stand Update Dyno Electrical System Diagram to Version 2.2 (created new connector numbers) Updated RW-3 Connector Master List Updated MCN Breakout Pinouts
</commit_message>
<xml_diff>
--- a/MCN Breakout Pinouts.xlsx
+++ b/MCN Breakout Pinouts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="132">
   <si>
     <t>5V</t>
   </si>
@@ -153,9 +153,6 @@
     <t>12V</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>DC-DC Temperature</t>
   </si>
   <si>
@@ -340,6 +337,81 @@
   </si>
   <si>
     <t>Rear CAN Backplane</t>
+  </si>
+  <si>
+    <t>X-340</t>
+  </si>
+  <si>
+    <t>X-206</t>
+  </si>
+  <si>
+    <t>X-207</t>
+  </si>
+  <si>
+    <t>X-339</t>
+  </si>
+  <si>
+    <t>X-336</t>
+  </si>
+  <si>
+    <t>X-337</t>
+  </si>
+  <si>
+    <t>X-413</t>
+  </si>
+  <si>
+    <t>X-329</t>
+  </si>
+  <si>
+    <t>X-203</t>
+  </si>
+  <si>
+    <t>X-205</t>
+  </si>
+  <si>
+    <t>X-202</t>
+  </si>
+  <si>
+    <t>X-201</t>
+  </si>
+  <si>
+    <t>Front Enclosure (CAN 2)</t>
+  </si>
+  <si>
+    <t>X-204</t>
+  </si>
+  <si>
+    <t>BMS (CAN 2)</t>
+  </si>
+  <si>
+    <t>X-321</t>
+  </si>
+  <si>
+    <t>X-322</t>
+  </si>
+  <si>
+    <t>X-320</t>
+  </si>
+  <si>
+    <t>X-319</t>
+  </si>
+  <si>
+    <t>X-318</t>
+  </si>
+  <si>
+    <t>X-317</t>
+  </si>
+  <si>
+    <t>X-316</t>
+  </si>
+  <si>
+    <t>X-314</t>
+  </si>
+  <si>
+    <t>X-315</t>
+  </si>
+  <si>
+    <t>X-313</t>
   </si>
 </sst>
 </file>
@@ -409,7 +481,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -423,15 +495,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -439,23 +505,26 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,14 +535,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -784,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +860,7 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="16" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -811,22 +877,22 @@
       <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>78</v>
+      <c r="E1" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="A2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -841,8 +907,8 @@
       <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>79</v>
+      <c r="E3" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>5</v>
@@ -857,8 +923,8 @@
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>80</v>
+      <c r="E4" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
@@ -870,11 +936,11 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>81</v>
+      <c r="D5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>5</v>
@@ -889,8 +955,8 @@
       <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>82</v>
+      <c r="E6" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>6</v>
@@ -905,7 +971,7 @@
       <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -917,7 +983,7 @@
       <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -933,7 +999,7 @@
       <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -949,14 +1015,14 @@
       <c r="D10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="5">
@@ -965,87 +1031,87 @@
       <c r="D11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>79</v>
+      <c r="E11" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>80</v>
+      <c r="E12" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5">
         <v>3</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>83</v>
+      <c r="E13" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>84</v>
+      <c r="E14" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5">
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>85</v>
+      <c r="E15" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5">
         <v>6</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1053,15 +1119,15 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="5">
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1069,15 +1135,15 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5">
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1097,8 +1163,8 @@
       <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>79</v>
+      <c r="E19" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>15</v>
@@ -1113,8 +1179,8 @@
       <c r="D20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>86</v>
+      <c r="E20" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>15</v>
@@ -1129,7 +1195,7 @@
       <c r="D21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1145,7 +1211,7 @@
       <c r="D22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1161,19 +1227,19 @@
       <c r="D23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>87</v>
+      <c r="E23" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>52</v>
+      <c r="A24" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1181,66 +1247,66 @@
       <c r="D24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>79</v>
+      <c r="E24" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="5">
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>88</v>
+      <c r="E25" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="5">
         <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="5">
         <v>4</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="A28" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
@@ -1255,8 +1321,8 @@
       <c r="D29" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>79</v>
+      <c r="E29" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>18</v>
@@ -1271,7 +1337,7 @@
       <c r="D30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F30" s="4" t="s">
@@ -1284,11 +1350,11 @@
       <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>81</v>
+      <c r="D31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>18</v>
@@ -1303,8 +1369,8 @@
       <c r="D32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>89</v>
+      <c r="E32" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>19</v>
@@ -1319,8 +1385,8 @@
       <c r="D33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>90</v>
+      <c r="E33" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>20</v>
@@ -1335,7 +1401,7 @@
       <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F34" s="4" t="s">
@@ -1348,13 +1414,13 @@
       <c r="C35" s="3">
         <v>7</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="9" t="s">
+      <c r="D35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1367,14 +1433,14 @@
       <c r="D36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="5">
@@ -1383,23 +1449,23 @@
       <c r="D37" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>79</v>
+      <c r="E37" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="5">
         <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F38" s="6" t="s">
@@ -1407,79 +1473,79 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="5">
         <v>3</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>82</v>
+      <c r="E39" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
       <c r="C40" s="5">
         <v>4</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>83</v>
+      <c r="E40" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="5">
         <v>5</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="16" t="s">
-        <v>84</v>
+      <c r="E41" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="5">
         <v>6</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>85</v>
+      <c r="E42" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="5">
         <v>7</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F43" s="6" t="s">
@@ -1487,15 +1553,15 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="5">
         <v>8</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -1515,8 +1581,8 @@
       <c r="D45" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="14" t="s">
-        <v>79</v>
+      <c r="E45" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>35</v>
@@ -1531,8 +1597,8 @@
       <c r="D46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>86</v>
+      <c r="E46" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>35</v>
@@ -1547,7 +1613,7 @@
       <c r="D47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -1563,8 +1629,8 @@
       <c r="D48" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="14" t="s">
-        <v>87</v>
+      <c r="E48" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>35</v>
@@ -1579,18 +1645,18 @@
       <c r="D49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>88</v>
+      <c r="E49" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="18" t="s">
         <v>27</v>
       </c>
       <c r="C50" s="5">
@@ -1599,39 +1665,39 @@
       <c r="D50" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>79</v>
+      <c r="E50" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="5">
         <v>2</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>91</v>
+      <c r="E51" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
       <c r="C52" s="5">
         <v>3</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F52" s="6" t="s">
@@ -1639,46 +1705,46 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="5">
         <v>4</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>92</v>
+      <c r="E53" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
       <c r="C54" s="5">
         <v>5</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>93</v>
+      <c r="E54" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
+      <c r="A55" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
@@ -1693,8 +1759,8 @@
       <c r="D56" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E56" s="14" t="s">
-        <v>79</v>
+      <c r="E56" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>41</v>
@@ -1709,8 +1775,8 @@
       <c r="D57" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="14" t="s">
-        <v>82</v>
+      <c r="E57" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>41</v>
@@ -1725,7 +1791,7 @@
       <c r="D58" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F58" s="4" t="s">
@@ -1733,10 +1799,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C59" s="5">
@@ -1745,39 +1811,39 @@
       <c r="D59" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="16" t="s">
-        <v>79</v>
+      <c r="E59" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
       <c r="C60" s="5">
         <v>2</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>81</v>
+      <c r="D60" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
       <c r="C61" s="5">
         <v>3</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F61" s="6" t="s">
@@ -1797,8 +1863,8 @@
       <c r="D62" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E62" s="14" t="s">
-        <v>79</v>
+      <c r="E62" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>43</v>
@@ -1813,8 +1879,8 @@
       <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="14" t="s">
-        <v>83</v>
+      <c r="E63" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>43</v>
@@ -1829,7 +1895,7 @@
       <c r="D64" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -1837,11 +1903,11 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>52</v>
+      <c r="A65" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="C65" s="5">
         <v>1</v>
@@ -1849,67 +1915,67 @@
       <c r="D65" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="5">
+        <v>2</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="5">
+        <v>3</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="5">
+        <v>4</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F65" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="5">
-        <v>2</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="5">
-        <v>3</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="23"/>
-      <c r="C68" s="5">
-        <v>4</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>50</v>
+      <c r="F68" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
-        <v>45</v>
+      <c r="A69" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C69" s="3">
         <v>1</v>
@@ -1917,11 +1983,11 @@
       <c r="D69" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="14" t="s">
-        <v>84</v>
+      <c r="E69" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1933,11 +1999,11 @@
       <c r="D70" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="14" t="s">
-        <v>85</v>
+      <c r="E70" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1949,11 +2015,11 @@
       <c r="D71" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="14" t="s">
-        <v>86</v>
+      <c r="E71" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,145 +2031,147 @@
       <c r="D72" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="23" t="s">
+      <c r="A73" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C73" s="5">
         <v>1</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="5">
+        <v>2</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F73" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="5">
-        <v>2</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F74" s="30"/>
+      <c r="F74" s="20"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="22"/>
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
       <c r="C75" s="5">
         <v>3</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F75" s="20"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="5">
+        <v>4</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F75" s="30"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="5">
-        <v>4</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F76" s="30"/>
+      <c r="F76" s="20"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
-      <c r="B77" s="22"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
       <c r="C77" s="5">
         <v>5</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F77" s="30"/>
+      <c r="D77" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F77" s="20"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78" s="22"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="5">
         <v>6</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="30"/>
+      <c r="D78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="20"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="22"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
       <c r="C79" s="5">
         <v>7</v>
       </c>
-      <c r="D79" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="30"/>
+      <c r="D79" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" s="20"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80" s="22"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
       <c r="C80" s="5">
         <v>8</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F80" s="30"/>
+      <c r="D80" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="20"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
+      <c r="A81" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B82" s="20" t="s">
+      <c r="A82" s="22" t="s">
         <v>98</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
@@ -2111,8 +2179,8 @@
       <c r="D82" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>79</v>
+      <c r="E82" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>18</v>
@@ -2127,7 +2195,7 @@
       <c r="D83" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F83" s="4" t="s">
@@ -2140,11 +2208,11 @@
       <c r="C84" s="3">
         <v>3</v>
       </c>
-      <c r="D84" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>81</v>
+      <c r="D84" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>18</v>
@@ -2159,8 +2227,8 @@
       <c r="D85" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E85" s="14" t="s">
-        <v>89</v>
+      <c r="E85" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>19</v>
@@ -2175,8 +2243,8 @@
       <c r="D86" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="14" t="s">
-        <v>90</v>
+      <c r="E86" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>20</v>
@@ -2191,7 +2259,7 @@
       <c r="D87" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F87" s="4" t="s">
@@ -2204,13 +2272,13 @@
       <c r="C88" s="3">
         <v>7</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E88" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F88" s="9" t="s">
+      <c r="D88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F88" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2220,13 +2288,13 @@
       <c r="C89" s="3">
         <v>8</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F89" s="9" t="s">
+      <c r="D89" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2236,13 +2304,13 @@
       <c r="C90" s="3">
         <v>9</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F90" s="9" t="s">
+      <c r="D90" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2255,15 +2323,15 @@
       <c r="D91" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E91" s="13"/>
+      <c r="E91" s="11"/>
       <c r="F91" s="4"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>98</v>
+      <c r="A92" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="C92" s="5">
         <v>1</v>
@@ -2271,167 +2339,167 @@
       <c r="D92" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E92" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>97</v>
+      <c r="E92" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
-      <c r="B93" s="22"/>
+      <c r="A93" s="17"/>
+      <c r="B93" s="18"/>
       <c r="C93" s="5">
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E93" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>97</v>
+      <c r="E93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
-      <c r="B94" s="22"/>
+      <c r="A94" s="17"/>
+      <c r="B94" s="18"/>
       <c r="C94" s="5">
         <v>3</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E94" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>97</v>
+      <c r="E94" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
-      <c r="B95" s="22"/>
+      <c r="A95" s="17"/>
+      <c r="B95" s="18"/>
       <c r="C95" s="5">
         <v>4</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E95" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>101</v>
+      <c r="E95" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
-      <c r="B96" s="22"/>
+      <c r="A96" s="17"/>
+      <c r="B96" s="18"/>
       <c r="C96" s="5">
         <v>5</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E96" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>101</v>
+      <c r="E96" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="23"/>
-      <c r="B97" s="22"/>
+      <c r="A97" s="17"/>
+      <c r="B97" s="18"/>
       <c r="C97" s="5">
         <v>6</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E97" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F97" s="8" t="s">
-        <v>101</v>
+      <c r="E97" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="23"/>
-      <c r="B98" s="22"/>
+      <c r="A98" s="17"/>
+      <c r="B98" s="18"/>
       <c r="C98" s="5">
         <v>7</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E98" s="15"/>
+      <c r="E98" s="13"/>
       <c r="F98" s="6"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="23"/>
-      <c r="B99" s="22"/>
+      <c r="A99" s="17"/>
+      <c r="B99" s="18"/>
       <c r="C99" s="5">
         <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E99" s="15"/>
+      <c r="E99" s="13"/>
       <c r="F99" s="6"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="23"/>
-      <c r="B100" s="22"/>
+      <c r="A100" s="17"/>
+      <c r="B100" s="18"/>
       <c r="C100" s="5">
         <v>9</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E100" s="15"/>
+      <c r="E100" s="13"/>
       <c r="F100" s="6"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="23"/>
-      <c r="B101" s="22"/>
+      <c r="A101" s="17"/>
+      <c r="B101" s="18"/>
       <c r="C101" s="5">
         <v>10</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E101" s="15"/>
+      <c r="E101" s="13"/>
       <c r="F101" s="6"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
+      <c r="A102" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="27"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="19"/>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19"/>
-      <c r="F102" s="19"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="B103" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C103" s="3">
         <v>1</v>
       </c>
-      <c r="D103" s="10" t="s">
+      <c r="D103" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E103" s="17"/>
-      <c r="F103" s="25" t="s">
-        <v>57</v>
+      <c r="E103" s="15"/>
+      <c r="F103" s="24" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2440,94 +2508,94 @@
       <c r="C104" s="3">
         <v>2</v>
       </c>
-      <c r="D104" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E104" s="17"/>
-      <c r="F104" s="25"/>
+      <c r="D104" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="15"/>
+      <c r="F104" s="24"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B105" s="23" t="s">
-        <v>105</v>
+      <c r="A105" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C105" s="5">
         <v>1</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="D105" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E105" s="14"/>
+      <c r="F105" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="18"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="5">
+        <v>2</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E106" s="14"/>
+      <c r="F106" s="26"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="18"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="5">
+        <v>3</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="14"/>
+      <c r="F107" s="26"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="18"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="5">
+        <v>4</v>
+      </c>
+      <c r="D108" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E105" s="16"/>
-      <c r="F105" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="5">
-        <v>2</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E106" s="16"/>
-      <c r="F106" s="27"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="22"/>
-      <c r="B107" s="22"/>
-      <c r="C107" s="5">
-        <v>3</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E107" s="16"/>
-      <c r="F107" s="27"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="22"/>
-      <c r="B108" s="22"/>
-      <c r="C108" s="5">
-        <v>4</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E108" s="16"/>
-      <c r="F108" s="27"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="26"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="22"/>
-      <c r="B109" s="22"/>
+      <c r="A109" s="18"/>
+      <c r="B109" s="18"/>
       <c r="C109" s="5">
         <v>5</v>
       </c>
-      <c r="D109" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E109" s="16"/>
-      <c r="F109" s="27"/>
+      <c r="D109" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E109" s="14"/>
+      <c r="F109" s="26"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="21" t="s">
-        <v>45</v>
+      <c r="A110" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E110" s="13"/>
-      <c r="F110" s="20" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="E110" s="11"/>
+      <c r="F110" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2539,7 +2607,7 @@
       <c r="D111" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E111" s="13"/>
+      <c r="E111" s="11"/>
       <c r="F111" s="21"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2551,7 +2619,7 @@
       <c r="D112" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E112" s="13"/>
+      <c r="E112" s="11"/>
       <c r="F112" s="21"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,9 +2629,9 @@
         <v>4</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E113" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="E113" s="11"/>
       <c r="F113" s="21"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2573,17 +2641,17 @@
         <v>5</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E114" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="E114" s="11"/>
       <c r="F114" s="21"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B115" s="22" t="s">
-        <v>49</v>
+      <c r="A115" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="C115" s="5">
         <v>1</v>
@@ -2591,97 +2659,97 @@
       <c r="D115" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E115" s="15"/>
-      <c r="F115" s="22" t="s">
-        <v>64</v>
+      <c r="E115" s="13"/>
+      <c r="F115" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="22"/>
-      <c r="B116" s="22"/>
+      <c r="A116" s="18"/>
+      <c r="B116" s="18"/>
       <c r="C116" s="5">
         <v>2</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E116" s="15"/>
-      <c r="F116" s="22"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="18"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="22"/>
-      <c r="B117" s="22"/>
+      <c r="A117" s="18"/>
+      <c r="B117" s="18"/>
       <c r="C117" s="5">
         <v>3</v>
       </c>
       <c r="D117" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E117" s="13"/>
+      <c r="F117" s="18"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="18"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="5">
+        <v>4</v>
+      </c>
+      <c r="D118" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E117" s="15"/>
-      <c r="F117" s="22"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="22"/>
-      <c r="B118" s="22"/>
-      <c r="C118" s="5">
-        <v>4</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E118" s="15"/>
-      <c r="F118" s="22"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="18"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="22"/>
-      <c r="B119" s="22"/>
+      <c r="A119" s="18"/>
+      <c r="B119" s="18"/>
       <c r="C119" s="5">
         <v>5</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E119" s="15"/>
-      <c r="F119" s="22"/>
+        <v>59</v>
+      </c>
+      <c r="E119" s="13"/>
+      <c r="F119" s="18"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="22"/>
-      <c r="B120" s="22"/>
+      <c r="A120" s="18"/>
+      <c r="B120" s="18"/>
       <c r="C120" s="5">
         <v>6</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E120" s="15"/>
-      <c r="F120" s="22"/>
+        <v>60</v>
+      </c>
+      <c r="E120" s="13"/>
+      <c r="F120" s="18"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B121" s="19"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
+      <c r="A121" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121" s="27"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="21" t="s">
-        <v>45</v>
+      <c r="A122" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C122" s="3">
         <v>1</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E122" s="13"/>
-      <c r="F122" s="28" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="E122" s="11"/>
+      <c r="F122" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2693,8 +2761,8 @@
       <c r="D123" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E123" s="13"/>
-      <c r="F123" s="25"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="24"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="21"/>
@@ -2705,8 +2773,8 @@
       <c r="D124" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E124" s="13"/>
-      <c r="F124" s="25"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="24"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
@@ -2715,10 +2783,10 @@
         <v>4</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E125" s="13"/>
-      <c r="F125" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E125" s="11"/>
+      <c r="F125" s="24"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
@@ -2727,93 +2795,93 @@
         <v>5</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E126" s="13"/>
-      <c r="F126" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E126" s="11"/>
+      <c r="F126" s="24"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B127" s="23" t="s">
-        <v>105</v>
+      <c r="A127" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C127" s="5">
         <v>1</v>
       </c>
-      <c r="D127" s="8" t="s">
+      <c r="D127" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" s="14"/>
+      <c r="F127" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="18"/>
+      <c r="B128" s="18"/>
+      <c r="C128" s="5">
+        <v>2</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E128" s="14"/>
+      <c r="F128" s="26"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="18"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="5">
+        <v>3</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="14"/>
+      <c r="F129" s="26"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="18"/>
+      <c r="B130" s="18"/>
+      <c r="C130" s="5">
+        <v>4</v>
+      </c>
+      <c r="D130" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E127" s="16"/>
-      <c r="F127" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="22"/>
-      <c r="B128" s="22"/>
-      <c r="C128" s="5">
-        <v>2</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E128" s="16"/>
-      <c r="F128" s="27"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="22"/>
-      <c r="B129" s="22"/>
-      <c r="C129" s="5">
-        <v>3</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" s="16"/>
-      <c r="F129" s="27"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="22"/>
-      <c r="B130" s="22"/>
-      <c r="C130" s="5">
-        <v>4</v>
-      </c>
-      <c r="D130" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E130" s="16"/>
-      <c r="F130" s="27"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="26"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="22"/>
-      <c r="B131" s="22"/>
+      <c r="A131" s="18"/>
+      <c r="B131" s="18"/>
       <c r="C131" s="5">
         <v>5</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E131" s="16"/>
-      <c r="F131" s="27"/>
+      <c r="D131" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E131" s="14"/>
+      <c r="F131" s="26"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="21" t="s">
-        <v>45</v>
+      <c r="A132" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="B132" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C132" s="3">
         <v>1</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E132" s="13"/>
-      <c r="F132" s="28" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="E132" s="11"/>
+      <c r="F132" s="23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -2825,8 +2893,8 @@
       <c r="D133" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E133" s="13"/>
-      <c r="F133" s="25"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="24"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
@@ -2837,8 +2905,8 @@
       <c r="D134" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E134" s="13"/>
-      <c r="F134" s="25"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="24"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="21"/>
@@ -2847,10 +2915,10 @@
         <v>4</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E135" s="13"/>
-      <c r="F135" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E135" s="11"/>
+      <c r="F135" s="24"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
@@ -2859,93 +2927,93 @@
         <v>5</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E136" s="13"/>
-      <c r="F136" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E136" s="11"/>
+      <c r="F136" s="24"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B137" s="23" t="s">
-        <v>105</v>
+      <c r="A137" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C137" s="5">
         <v>1</v>
       </c>
-      <c r="D137" s="8" t="s">
+      <c r="D137" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E137" s="14"/>
+      <c r="F137" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="18"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="5">
+        <v>2</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E138" s="14"/>
+      <c r="F138" s="26"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="18"/>
+      <c r="B139" s="18"/>
+      <c r="C139" s="5">
+        <v>3</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E139" s="14"/>
+      <c r="F139" s="26"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="18"/>
+      <c r="B140" s="18"/>
+      <c r="C140" s="5">
+        <v>4</v>
+      </c>
+      <c r="D140" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E137" s="16"/>
-      <c r="F137" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="22"/>
-      <c r="B138" s="22"/>
-      <c r="C138" s="5">
-        <v>2</v>
-      </c>
-      <c r="D138" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E138" s="16"/>
-      <c r="F138" s="27"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="22"/>
-      <c r="B139" s="22"/>
-      <c r="C139" s="5">
-        <v>3</v>
-      </c>
-      <c r="D139" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E139" s="16"/>
-      <c r="F139" s="27"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="22"/>
-      <c r="B140" s="22"/>
-      <c r="C140" s="5">
-        <v>4</v>
-      </c>
-      <c r="D140" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E140" s="16"/>
-      <c r="F140" s="27"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="26"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="22"/>
-      <c r="B141" s="22"/>
+      <c r="A141" s="18"/>
+      <c r="B141" s="18"/>
       <c r="C141" s="5">
         <v>5</v>
       </c>
-      <c r="D141" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E141" s="16"/>
-      <c r="F141" s="27"/>
+      <c r="D141" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E141" s="14"/>
+      <c r="F141" s="26"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="21" t="s">
-        <v>45</v>
+      <c r="A142" s="22" t="s">
+        <v>120</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C142" s="3">
         <v>1</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E142" s="13"/>
-      <c r="F142" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="E142" s="11"/>
+      <c r="F142" s="23" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -2957,8 +3025,8 @@
       <c r="D143" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E143" s="13"/>
-      <c r="F143" s="25"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="24"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="21"/>
@@ -2969,8 +3037,8 @@
       <c r="D144" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E144" s="13"/>
-      <c r="F144" s="25"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="24"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="21"/>
@@ -2979,10 +3047,10 @@
         <v>4</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E145" s="13"/>
-      <c r="F145" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E145" s="11"/>
+      <c r="F145" s="24"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="21"/>
@@ -2991,95 +3059,95 @@
         <v>5</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E146" s="13"/>
-      <c r="F146" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E146" s="11"/>
+      <c r="F146" s="24"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B147" s="23" t="s">
-        <v>49</v>
+      <c r="A147" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C147" s="5">
         <v>1</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="D147" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E147" s="16"/>
-      <c r="F147" s="26" t="s">
-        <v>68</v>
+      <c r="E147" s="14"/>
+      <c r="F147" s="25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="22"/>
-      <c r="B148" s="22"/>
+      <c r="A148" s="18"/>
+      <c r="B148" s="18"/>
       <c r="C148" s="5">
         <v>2</v>
       </c>
-      <c r="D148" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E148" s="16"/>
-      <c r="F148" s="27"/>
+      <c r="D148" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E148" s="14"/>
+      <c r="F148" s="26"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="22"/>
-      <c r="B149" s="22"/>
+      <c r="A149" s="18"/>
+      <c r="B149" s="18"/>
       <c r="C149" s="5">
         <v>3</v>
       </c>
-      <c r="D149" s="8" t="s">
+      <c r="D149" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E149" s="14"/>
+      <c r="F149" s="26"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="18"/>
+      <c r="B150" s="18"/>
+      <c r="C150" s="5">
+        <v>4</v>
+      </c>
+      <c r="D150" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E149" s="16"/>
-      <c r="F149" s="27"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="22"/>
-      <c r="B150" s="22"/>
-      <c r="C150" s="5">
-        <v>4</v>
-      </c>
-      <c r="D150" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E150" s="16"/>
-      <c r="F150" s="27"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="26"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="22"/>
-      <c r="B151" s="22"/>
+      <c r="A151" s="18"/>
+      <c r="B151" s="18"/>
       <c r="C151" s="5">
         <v>5</v>
       </c>
-      <c r="D151" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E151" s="16"/>
-      <c r="F151" s="27"/>
+      <c r="D151" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E151" s="14"/>
+      <c r="F151" s="26"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="22"/>
-      <c r="B152" s="22"/>
+      <c r="A152" s="18"/>
+      <c r="B152" s="18"/>
       <c r="C152" s="5">
         <v>6</v>
       </c>
-      <c r="D152" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E152" s="16"/>
-      <c r="F152" s="27"/>
+      <c r="D152" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E152" s="14"/>
+      <c r="F152" s="26"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B153" s="20" t="s">
-        <v>49</v>
+      <c r="A153" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B153" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="C153" s="3">
         <v>1</v>
@@ -3087,9 +3155,9 @@
       <c r="D153" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E153" s="13"/>
-      <c r="F153" s="28" t="s">
-        <v>69</v>
+      <c r="E153" s="11"/>
+      <c r="F153" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -3101,8 +3169,8 @@
       <c r="D154" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E154" s="13"/>
-      <c r="F154" s="25"/>
+      <c r="E154" s="11"/>
+      <c r="F154" s="24"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="21"/>
@@ -3111,10 +3179,10 @@
         <v>3</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E155" s="13"/>
-      <c r="F155" s="25"/>
+        <v>57</v>
+      </c>
+      <c r="E155" s="11"/>
+      <c r="F155" s="24"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="21"/>
@@ -3123,10 +3191,10 @@
         <v>4</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E156" s="13"/>
-      <c r="F156" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E156" s="11"/>
+      <c r="F156" s="24"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="21"/>
@@ -3135,10 +3203,10 @@
         <v>5</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E157" s="13"/>
-      <c r="F157" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E157" s="11"/>
+      <c r="F157" s="24"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="21"/>
@@ -3147,95 +3215,95 @@
         <v>6</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E158" s="13"/>
-      <c r="F158" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="E158" s="11"/>
+      <c r="F158" s="24"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B159" s="23" t="s">
-        <v>49</v>
+      <c r="A159" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B159" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C159" s="5">
         <v>1</v>
       </c>
-      <c r="D159" s="8" t="s">
+      <c r="D159" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E159" s="16"/>
-      <c r="F159" s="26" t="s">
-        <v>70</v>
+      <c r="E159" s="14"/>
+      <c r="F159" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="22"/>
-      <c r="B160" s="22"/>
+      <c r="A160" s="18"/>
+      <c r="B160" s="18"/>
       <c r="C160" s="5">
         <v>2</v>
       </c>
-      <c r="D160" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E160" s="16"/>
-      <c r="F160" s="27"/>
+      <c r="D160" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E160" s="14"/>
+      <c r="F160" s="26"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="22"/>
-      <c r="B161" s="22"/>
+      <c r="A161" s="18"/>
+      <c r="B161" s="18"/>
       <c r="C161" s="5">
         <v>3</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="D161" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E161" s="14"/>
+      <c r="F161" s="26"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="18"/>
+      <c r="B162" s="18"/>
+      <c r="C162" s="5">
+        <v>4</v>
+      </c>
+      <c r="D162" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E161" s="16"/>
-      <c r="F161" s="27"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="22"/>
-      <c r="B162" s="22"/>
-      <c r="C162" s="5">
-        <v>4</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E162" s="16"/>
-      <c r="F162" s="27"/>
+      <c r="E162" s="14"/>
+      <c r="F162" s="26"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="22"/>
-      <c r="B163" s="22"/>
+      <c r="A163" s="18"/>
+      <c r="B163" s="18"/>
       <c r="C163" s="5">
         <v>5</v>
       </c>
-      <c r="D163" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E163" s="16"/>
-      <c r="F163" s="27"/>
+      <c r="D163" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E163" s="14"/>
+      <c r="F163" s="26"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="22"/>
-      <c r="B164" s="22"/>
+      <c r="A164" s="18"/>
+      <c r="B164" s="18"/>
       <c r="C164" s="5">
         <v>6</v>
       </c>
-      <c r="D164" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E164" s="16"/>
-      <c r="F164" s="27"/>
+      <c r="D164" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E164" s="14"/>
+      <c r="F164" s="26"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B165" s="20" t="s">
-        <v>49</v>
+      <c r="A165" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B165" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="C165" s="3">
         <v>1</v>
@@ -3243,9 +3311,9 @@
       <c r="D165" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E165" s="13"/>
-      <c r="F165" s="28" t="s">
-        <v>71</v>
+      <c r="E165" s="11"/>
+      <c r="F165" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3257,8 +3325,8 @@
       <c r="D166" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E166" s="13"/>
-      <c r="F166" s="25"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="24"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="21"/>
@@ -3267,10 +3335,10 @@
         <v>3</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E167" s="13"/>
-      <c r="F167" s="25"/>
+        <v>57</v>
+      </c>
+      <c r="E167" s="11"/>
+      <c r="F167" s="24"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="21"/>
@@ -3279,10 +3347,10 @@
         <v>4</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E168" s="13"/>
-      <c r="F168" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E168" s="11"/>
+      <c r="F168" s="24"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="21"/>
@@ -3291,10 +3359,10 @@
         <v>5</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E169" s="13"/>
-      <c r="F169" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E169" s="11"/>
+      <c r="F169" s="24"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="21"/>
@@ -3303,95 +3371,95 @@
         <v>6</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E170" s="13"/>
-      <c r="F170" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="E170" s="11"/>
+      <c r="F170" s="24"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B171" s="23" t="s">
-        <v>49</v>
+      <c r="A171" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B171" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C171" s="5">
         <v>1</v>
       </c>
-      <c r="D171" s="8" t="s">
+      <c r="D171" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E171" s="16"/>
-      <c r="F171" s="26" t="s">
-        <v>72</v>
+      <c r="E171" s="14"/>
+      <c r="F171" s="25" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="22"/>
-      <c r="B172" s="22"/>
+      <c r="A172" s="18"/>
+      <c r="B172" s="18"/>
       <c r="C172" s="5">
         <v>2</v>
       </c>
-      <c r="D172" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E172" s="16"/>
-      <c r="F172" s="27"/>
+      <c r="D172" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E172" s="14"/>
+      <c r="F172" s="26"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="22"/>
-      <c r="B173" s="22"/>
+      <c r="A173" s="18"/>
+      <c r="B173" s="18"/>
       <c r="C173" s="5">
         <v>3</v>
       </c>
-      <c r="D173" s="8" t="s">
+      <c r="D173" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E173" s="14"/>
+      <c r="F173" s="26"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="18"/>
+      <c r="B174" s="18"/>
+      <c r="C174" s="5">
+        <v>4</v>
+      </c>
+      <c r="D174" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E173" s="16"/>
-      <c r="F173" s="27"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="22"/>
-      <c r="B174" s="22"/>
-      <c r="C174" s="5">
-        <v>4</v>
-      </c>
-      <c r="D174" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E174" s="16"/>
-      <c r="F174" s="27"/>
+      <c r="E174" s="14"/>
+      <c r="F174" s="26"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="22"/>
-      <c r="B175" s="22"/>
+      <c r="A175" s="18"/>
+      <c r="B175" s="18"/>
       <c r="C175" s="5">
         <v>5</v>
       </c>
-      <c r="D175" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E175" s="16"/>
-      <c r="F175" s="27"/>
+      <c r="D175" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E175" s="14"/>
+      <c r="F175" s="26"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="22"/>
-      <c r="B176" s="22"/>
+      <c r="A176" s="18"/>
+      <c r="B176" s="18"/>
       <c r="C176" s="5">
         <v>6</v>
       </c>
-      <c r="D176" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E176" s="16"/>
-      <c r="F176" s="27"/>
+      <c r="D176" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E176" s="14"/>
+      <c r="F176" s="26"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B177" s="20" t="s">
-        <v>49</v>
+      <c r="A177" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B177" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="C177" s="3">
         <v>1</v>
@@ -3399,9 +3467,9 @@
       <c r="D177" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E177" s="13"/>
-      <c r="F177" s="28" t="s">
-        <v>73</v>
+      <c r="E177" s="11"/>
+      <c r="F177" s="23" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3413,8 +3481,8 @@
       <c r="D178" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E178" s="13"/>
-      <c r="F178" s="25"/>
+      <c r="E178" s="11"/>
+      <c r="F178" s="24"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="21"/>
@@ -3423,10 +3491,10 @@
         <v>3</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E179" s="13"/>
-      <c r="F179" s="25"/>
+        <v>57</v>
+      </c>
+      <c r="E179" s="11"/>
+      <c r="F179" s="24"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="21"/>
@@ -3435,10 +3503,10 @@
         <v>4</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E180" s="13"/>
-      <c r="F180" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E180" s="11"/>
+      <c r="F180" s="24"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="21"/>
@@ -3447,10 +3515,10 @@
         <v>5</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E181" s="13"/>
-      <c r="F181" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E181" s="11"/>
+      <c r="F181" s="24"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="21"/>
@@ -3459,95 +3527,95 @@
         <v>6</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E182" s="13"/>
-      <c r="F182" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="E182" s="11"/>
+      <c r="F182" s="24"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B183" s="23" t="s">
-        <v>49</v>
+      <c r="A183" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B183" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C183" s="5">
         <v>1</v>
       </c>
-      <c r="D183" s="8" t="s">
+      <c r="D183" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E183" s="16"/>
-      <c r="F183" s="26" t="s">
-        <v>74</v>
+      <c r="E183" s="14"/>
+      <c r="F183" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="22"/>
-      <c r="B184" s="22"/>
+      <c r="A184" s="18"/>
+      <c r="B184" s="18"/>
       <c r="C184" s="5">
         <v>2</v>
       </c>
-      <c r="D184" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E184" s="16"/>
-      <c r="F184" s="27"/>
+      <c r="D184" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E184" s="14"/>
+      <c r="F184" s="26"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="22"/>
-      <c r="B185" s="22"/>
+      <c r="A185" s="18"/>
+      <c r="B185" s="18"/>
       <c r="C185" s="5">
         <v>3</v>
       </c>
-      <c r="D185" s="8" t="s">
+      <c r="D185" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E185" s="14"/>
+      <c r="F185" s="26"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="18"/>
+      <c r="B186" s="18"/>
+      <c r="C186" s="5">
+        <v>4</v>
+      </c>
+      <c r="D186" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E185" s="16"/>
-      <c r="F185" s="27"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="22"/>
-      <c r="B186" s="22"/>
-      <c r="C186" s="5">
-        <v>4</v>
-      </c>
-      <c r="D186" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E186" s="16"/>
-      <c r="F186" s="27"/>
+      <c r="E186" s="14"/>
+      <c r="F186" s="26"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="22"/>
-      <c r="B187" s="22"/>
+      <c r="A187" s="18"/>
+      <c r="B187" s="18"/>
       <c r="C187" s="5">
         <v>5</v>
       </c>
-      <c r="D187" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E187" s="16"/>
-      <c r="F187" s="27"/>
+      <c r="D187" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E187" s="14"/>
+      <c r="F187" s="26"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="22"/>
-      <c r="B188" s="22"/>
+      <c r="A188" s="18"/>
+      <c r="B188" s="18"/>
       <c r="C188" s="5">
         <v>6</v>
       </c>
-      <c r="D188" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E188" s="16"/>
-      <c r="F188" s="27"/>
+      <c r="D188" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E188" s="14"/>
+      <c r="F188" s="26"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B189" s="20" t="s">
-        <v>49</v>
+      <c r="A189" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B189" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="C189" s="3">
         <v>1</v>
@@ -3555,9 +3623,9 @@
       <c r="D189" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E189" s="13"/>
-      <c r="F189" s="28" t="s">
-        <v>75</v>
+      <c r="E189" s="11"/>
+      <c r="F189" s="23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -3569,8 +3637,8 @@
       <c r="D190" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E190" s="13"/>
-      <c r="F190" s="25"/>
+      <c r="E190" s="11"/>
+      <c r="F190" s="24"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="21"/>
@@ -3579,10 +3647,10 @@
         <v>3</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E191" s="13"/>
-      <c r="F191" s="25"/>
+        <v>57</v>
+      </c>
+      <c r="E191" s="11"/>
+      <c r="F191" s="24"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="21"/>
@@ -3591,10 +3659,10 @@
         <v>4</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E192" s="13"/>
-      <c r="F192" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E192" s="11"/>
+      <c r="F192" s="24"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="21"/>
@@ -3603,10 +3671,10 @@
         <v>5</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E193" s="13"/>
-      <c r="F193" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E193" s="11"/>
+      <c r="F193" s="24"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="21"/>
@@ -3615,95 +3683,95 @@
         <v>6</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E194" s="13"/>
-      <c r="F194" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="E194" s="11"/>
+      <c r="F194" s="24"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B195" s="23" t="s">
-        <v>49</v>
+      <c r="A195" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B195" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C195" s="5">
         <v>1</v>
       </c>
-      <c r="D195" s="8" t="s">
+      <c r="D195" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E195" s="16"/>
-      <c r="F195" s="26" t="s">
-        <v>76</v>
+      <c r="E195" s="14"/>
+      <c r="F195" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="22"/>
-      <c r="B196" s="22"/>
+      <c r="A196" s="18"/>
+      <c r="B196" s="18"/>
       <c r="C196" s="5">
         <v>2</v>
       </c>
-      <c r="D196" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E196" s="16"/>
-      <c r="F196" s="27"/>
+      <c r="D196" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E196" s="14"/>
+      <c r="F196" s="26"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="22"/>
-      <c r="B197" s="22"/>
+      <c r="A197" s="18"/>
+      <c r="B197" s="18"/>
       <c r="C197" s="5">
         <v>3</v>
       </c>
-      <c r="D197" s="8" t="s">
+      <c r="D197" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E197" s="14"/>
+      <c r="F197" s="26"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="18"/>
+      <c r="B198" s="18"/>
+      <c r="C198" s="5">
+        <v>4</v>
+      </c>
+      <c r="D198" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="16"/>
-      <c r="F197" s="27"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="22"/>
-      <c r="B198" s="22"/>
-      <c r="C198" s="5">
-        <v>4</v>
-      </c>
-      <c r="D198" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E198" s="16"/>
-      <c r="F198" s="27"/>
+      <c r="E198" s="14"/>
+      <c r="F198" s="26"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="22"/>
-      <c r="B199" s="22"/>
+      <c r="A199" s="18"/>
+      <c r="B199" s="18"/>
       <c r="C199" s="5">
         <v>5</v>
       </c>
-      <c r="D199" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E199" s="16"/>
-      <c r="F199" s="27"/>
+      <c r="D199" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E199" s="14"/>
+      <c r="F199" s="26"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="22"/>
-      <c r="B200" s="22"/>
+      <c r="A200" s="18"/>
+      <c r="B200" s="18"/>
       <c r="C200" s="5">
         <v>6</v>
       </c>
-      <c r="D200" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E200" s="16"/>
-      <c r="F200" s="27"/>
+      <c r="D200" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E200" s="14"/>
+      <c r="F200" s="26"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B201" s="20" t="s">
-        <v>56</v>
+      <c r="A201" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B201" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="C201" s="3">
         <v>1</v>
@@ -3711,22 +3779,22 @@
       <c r="D201" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E201" s="13"/>
-      <c r="F201" s="28" t="s">
-        <v>77</v>
+      <c r="E201" s="11"/>
+      <c r="F201" s="23" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="21"/>
-      <c r="B202" s="20"/>
+      <c r="B202" s="22"/>
       <c r="C202" s="3">
         <v>2</v>
       </c>
       <c r="D202" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E202" s="13"/>
-      <c r="F202" s="28"/>
+      <c r="E202" s="11"/>
+      <c r="F202" s="23"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C203"/>
@@ -3741,7 +3809,87 @@
       <c r="C206"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
+  <mergeCells count="96">
+    <mergeCell ref="A73:A80"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="A82:A91"/>
+    <mergeCell ref="B82:B91"/>
+    <mergeCell ref="B92:B101"/>
+    <mergeCell ref="A92:A101"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="F105:F109"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="B105:B109"/>
+    <mergeCell ref="A110:A114"/>
+    <mergeCell ref="B110:B114"/>
+    <mergeCell ref="F110:F114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="F115:F120"/>
+    <mergeCell ref="A121:F121"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="F122:F126"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="F127:F131"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="F132:F136"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="F137:F141"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="B147:B152"/>
+    <mergeCell ref="F147:F152"/>
+    <mergeCell ref="A153:A158"/>
+    <mergeCell ref="B153:B158"/>
+    <mergeCell ref="F153:F158"/>
+    <mergeCell ref="A159:A164"/>
+    <mergeCell ref="B159:B164"/>
+    <mergeCell ref="F159:F164"/>
+    <mergeCell ref="F183:F188"/>
+    <mergeCell ref="A165:A170"/>
+    <mergeCell ref="B165:B170"/>
+    <mergeCell ref="F165:F170"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="B171:B176"/>
+    <mergeCell ref="F171:F176"/>
     <mergeCell ref="B73:B80"/>
     <mergeCell ref="F73:F80"/>
     <mergeCell ref="A201:A202"/>
@@ -3758,85 +3906,6 @@
     <mergeCell ref="F177:F182"/>
     <mergeCell ref="A183:A188"/>
     <mergeCell ref="B183:B188"/>
-    <mergeCell ref="F183:F188"/>
-    <mergeCell ref="A165:A170"/>
-    <mergeCell ref="B165:B170"/>
-    <mergeCell ref="F165:F170"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="B171:B176"/>
-    <mergeCell ref="F171:F176"/>
-    <mergeCell ref="A153:A158"/>
-    <mergeCell ref="B153:B158"/>
-    <mergeCell ref="F153:F158"/>
-    <mergeCell ref="A159:A164"/>
-    <mergeCell ref="B159:B164"/>
-    <mergeCell ref="F159:F164"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="F142:F146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="B147:B152"/>
-    <mergeCell ref="F147:F152"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="F132:F136"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="F137:F141"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A122:A126"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="F122:F126"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="F127:F131"/>
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="B110:B114"/>
-    <mergeCell ref="F110:F114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="B115:B120"/>
-    <mergeCell ref="F115:F120"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="F105:F109"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="B105:B109"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="B37:B44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A81:F81"/>
-    <mergeCell ref="A82:A91"/>
-    <mergeCell ref="B82:B91"/>
-    <mergeCell ref="B92:B101"/>
-    <mergeCell ref="A92:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added pinout drawings for Dyno Stand
</commit_message>
<xml_diff>
--- a/MCN Breakout Pinouts.xlsx
+++ b/MCN Breakout Pinouts.xlsx
@@ -511,20 +511,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -535,11 +532,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="A205" sqref="A205"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,14 +885,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1176,8 +1176,8 @@
       <c r="C20" s="3">
         <v>2</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>2</v>
+      <c r="D20" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>85</v>
@@ -1299,14 +1299,14 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
@@ -1737,14 +1737,14 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
@@ -1971,7 +1971,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="20" t="s">
         <v>112</v>
       </c>
       <c r="B69" s="21" t="s">
@@ -2054,7 +2054,7 @@
       <c r="E73" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F73" s="19" t="s">
+      <c r="F73" s="27" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       <c r="E74" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F74" s="20"/>
+      <c r="F74" s="28"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="18"/>
@@ -2084,7 +2084,7 @@
       <c r="E75" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F75" s="20"/>
+      <c r="F75" s="28"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="18"/>
@@ -2098,7 +2098,7 @@
       <c r="E76" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F76" s="20"/>
+      <c r="F76" s="28"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="18"/>
@@ -2112,7 +2112,7 @@
       <c r="E77" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F77" s="20"/>
+      <c r="F77" s="28"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="18"/>
@@ -2126,7 +2126,7 @@
       <c r="E78" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="20"/>
+      <c r="F78" s="28"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="18"/>
@@ -2140,7 +2140,7 @@
       <c r="E79" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F79" s="20"/>
+      <c r="F79" s="28"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="18"/>
@@ -2154,23 +2154,23 @@
       <c r="E80" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="20"/>
+      <c r="F80" s="28"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="20" t="s">
         <v>97</v>
       </c>
       <c r="C82" s="3">
@@ -2475,17 +2475,17 @@
       <c r="F101" s="6"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="27" t="s">
+      <c r="A102" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="22" t="s">
+      <c r="A103" s="20" t="s">
         <v>107</v>
       </c>
       <c r="B103" s="21" t="s">
@@ -2498,7 +2498,7 @@
         <v>44</v>
       </c>
       <c r="E103" s="15"/>
-      <c r="F103" s="24" t="s">
+      <c r="F103" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
         <v>4</v>
       </c>
       <c r="E104" s="15"/>
-      <c r="F104" s="24"/>
+      <c r="F104" s="23"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
@@ -2528,7 +2528,7 @@
         <v>57</v>
       </c>
       <c r="E105" s="14"/>
-      <c r="F105" s="25" t="s">
+      <c r="F105" s="24" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2542,7 +2542,7 @@
         <v>44</v>
       </c>
       <c r="E106" s="14"/>
-      <c r="F106" s="26"/>
+      <c r="F106" s="25"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="18"/>
@@ -2554,7 +2554,7 @@
         <v>4</v>
       </c>
       <c r="E107" s="14"/>
-      <c r="F107" s="26"/>
+      <c r="F107" s="25"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="18"/>
@@ -2566,7 +2566,7 @@
         <v>58</v>
       </c>
       <c r="E108" s="14"/>
-      <c r="F108" s="26"/>
+      <c r="F108" s="25"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="18"/>
@@ -2578,10 +2578,10 @@
         <v>59</v>
       </c>
       <c r="E109" s="14"/>
-      <c r="F109" s="26"/>
+      <c r="F109" s="25"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="20" t="s">
         <v>109</v>
       </c>
       <c r="B110" s="21" t="s">
@@ -2594,7 +2594,7 @@
         <v>57</v>
       </c>
       <c r="E110" s="11"/>
-      <c r="F110" s="22" t="s">
+      <c r="F110" s="20" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2725,17 +2725,17 @@
       <c r="F120" s="18"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="27" t="s">
+      <c r="A121" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B121" s="27"/>
-      <c r="C121" s="27"/>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="27"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="22" t="s">
+      <c r="A122" s="20" t="s">
         <v>115</v>
       </c>
       <c r="B122" s="21" t="s">
@@ -2748,7 +2748,7 @@
         <v>57</v>
       </c>
       <c r="E122" s="11"/>
-      <c r="F122" s="23" t="s">
+      <c r="F122" s="26" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2762,7 +2762,7 @@
         <v>44</v>
       </c>
       <c r="E123" s="11"/>
-      <c r="F123" s="24"/>
+      <c r="F123" s="23"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="21"/>
@@ -2774,7 +2774,7 @@
         <v>4</v>
       </c>
       <c r="E124" s="11"/>
-      <c r="F124" s="24"/>
+      <c r="F124" s="23"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
@@ -2786,7 +2786,7 @@
         <v>58</v>
       </c>
       <c r="E125" s="11"/>
-      <c r="F125" s="24"/>
+      <c r="F125" s="23"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
@@ -2798,7 +2798,7 @@
         <v>59</v>
       </c>
       <c r="E126" s="11"/>
-      <c r="F126" s="24"/>
+      <c r="F126" s="23"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
@@ -2814,7 +2814,7 @@
         <v>57</v>
       </c>
       <c r="E127" s="14"/>
-      <c r="F127" s="25" t="s">
+      <c r="F127" s="24" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2828,7 +2828,7 @@
         <v>44</v>
       </c>
       <c r="E128" s="14"/>
-      <c r="F128" s="26"/>
+      <c r="F128" s="25"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="18"/>
@@ -2840,7 +2840,7 @@
         <v>4</v>
       </c>
       <c r="E129" s="14"/>
-      <c r="F129" s="26"/>
+      <c r="F129" s="25"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="18"/>
@@ -2852,7 +2852,7 @@
         <v>58</v>
       </c>
       <c r="E130" s="14"/>
-      <c r="F130" s="26"/>
+      <c r="F130" s="25"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="18"/>
@@ -2864,10 +2864,10 @@
         <v>59</v>
       </c>
       <c r="E131" s="14"/>
-      <c r="F131" s="26"/>
+      <c r="F131" s="25"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="22" t="s">
+      <c r="A132" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B132" s="21" t="s">
@@ -2880,7 +2880,7 @@
         <v>57</v>
       </c>
       <c r="E132" s="11"/>
-      <c r="F132" s="23" t="s">
+      <c r="F132" s="26" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2894,7 +2894,7 @@
         <v>44</v>
       </c>
       <c r="E133" s="11"/>
-      <c r="F133" s="24"/>
+      <c r="F133" s="23"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
@@ -2906,7 +2906,7 @@
         <v>4</v>
       </c>
       <c r="E134" s="11"/>
-      <c r="F134" s="24"/>
+      <c r="F134" s="23"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="21"/>
@@ -2918,7 +2918,7 @@
         <v>58</v>
       </c>
       <c r="E135" s="11"/>
-      <c r="F135" s="24"/>
+      <c r="F135" s="23"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
@@ -2930,7 +2930,7 @@
         <v>59</v>
       </c>
       <c r="E136" s="11"/>
-      <c r="F136" s="24"/>
+      <c r="F136" s="23"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
@@ -2946,7 +2946,7 @@
         <v>57</v>
       </c>
       <c r="E137" s="14"/>
-      <c r="F137" s="25" t="s">
+      <c r="F137" s="24" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2960,7 +2960,7 @@
         <v>44</v>
       </c>
       <c r="E138" s="14"/>
-      <c r="F138" s="26"/>
+      <c r="F138" s="25"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="18"/>
@@ -2972,7 +2972,7 @@
         <v>4</v>
       </c>
       <c r="E139" s="14"/>
-      <c r="F139" s="26"/>
+      <c r="F139" s="25"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="18"/>
@@ -2984,7 +2984,7 @@
         <v>58</v>
       </c>
       <c r="E140" s="14"/>
-      <c r="F140" s="26"/>
+      <c r="F140" s="25"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="18"/>
@@ -2996,10 +2996,10 @@
         <v>59</v>
       </c>
       <c r="E141" s="14"/>
-      <c r="F141" s="26"/>
+      <c r="F141" s="25"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="22" t="s">
+      <c r="A142" s="20" t="s">
         <v>120</v>
       </c>
       <c r="B142" s="21" t="s">
@@ -3012,7 +3012,7 @@
         <v>57</v>
       </c>
       <c r="E142" s="11"/>
-      <c r="F142" s="23" t="s">
+      <c r="F142" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
         <v>44</v>
       </c>
       <c r="E143" s="11"/>
-      <c r="F143" s="24"/>
+      <c r="F143" s="23"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="21"/>
@@ -3038,7 +3038,7 @@
         <v>4</v>
       </c>
       <c r="E144" s="11"/>
-      <c r="F144" s="24"/>
+      <c r="F144" s="23"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="21"/>
@@ -3050,7 +3050,7 @@
         <v>58</v>
       </c>
       <c r="E145" s="11"/>
-      <c r="F145" s="24"/>
+      <c r="F145" s="23"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="21"/>
@@ -3062,7 +3062,7 @@
         <v>59</v>
       </c>
       <c r="E146" s="11"/>
-      <c r="F146" s="24"/>
+      <c r="F146" s="23"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
@@ -3078,7 +3078,7 @@
         <v>44</v>
       </c>
       <c r="E147" s="14"/>
-      <c r="F147" s="25" t="s">
+      <c r="F147" s="24" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3092,7 +3092,7 @@
         <v>4</v>
       </c>
       <c r="E148" s="14"/>
-      <c r="F148" s="26"/>
+      <c r="F148" s="25"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="18"/>
@@ -3104,7 +3104,7 @@
         <v>57</v>
       </c>
       <c r="E149" s="14"/>
-      <c r="F149" s="26"/>
+      <c r="F149" s="25"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="18"/>
@@ -3116,7 +3116,7 @@
         <v>58</v>
       </c>
       <c r="E150" s="14"/>
-      <c r="F150" s="26"/>
+      <c r="F150" s="25"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="18"/>
@@ -3128,7 +3128,7 @@
         <v>59</v>
       </c>
       <c r="E151" s="14"/>
-      <c r="F151" s="26"/>
+      <c r="F151" s="25"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="18"/>
@@ -3140,13 +3140,13 @@
         <v>60</v>
       </c>
       <c r="E152" s="14"/>
-      <c r="F152" s="26"/>
+      <c r="F152" s="25"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="22" t="s">
+      <c r="A153" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B153" s="22" t="s">
+      <c r="B153" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C153" s="3">
@@ -3156,7 +3156,7 @@
         <v>44</v>
       </c>
       <c r="E153" s="11"/>
-      <c r="F153" s="23" t="s">
+      <c r="F153" s="26" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3170,7 +3170,7 @@
         <v>4</v>
       </c>
       <c r="E154" s="11"/>
-      <c r="F154" s="24"/>
+      <c r="F154" s="23"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="21"/>
@@ -3182,7 +3182,7 @@
         <v>57</v>
       </c>
       <c r="E155" s="11"/>
-      <c r="F155" s="24"/>
+      <c r="F155" s="23"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="21"/>
@@ -3194,7 +3194,7 @@
         <v>58</v>
       </c>
       <c r="E156" s="11"/>
-      <c r="F156" s="24"/>
+      <c r="F156" s="23"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="21"/>
@@ -3206,7 +3206,7 @@
         <v>59</v>
       </c>
       <c r="E157" s="11"/>
-      <c r="F157" s="24"/>
+      <c r="F157" s="23"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="21"/>
@@ -3218,7 +3218,7 @@
         <v>60</v>
       </c>
       <c r="E158" s="11"/>
-      <c r="F158" s="24"/>
+      <c r="F158" s="23"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="17" t="s">
@@ -3234,7 +3234,7 @@
         <v>44</v>
       </c>
       <c r="E159" s="14"/>
-      <c r="F159" s="25" t="s">
+      <c r="F159" s="24" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3248,7 +3248,7 @@
         <v>4</v>
       </c>
       <c r="E160" s="14"/>
-      <c r="F160" s="26"/>
+      <c r="F160" s="25"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="18"/>
@@ -3260,7 +3260,7 @@
         <v>57</v>
       </c>
       <c r="E161" s="14"/>
-      <c r="F161" s="26"/>
+      <c r="F161" s="25"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="18"/>
@@ -3272,7 +3272,7 @@
         <v>58</v>
       </c>
       <c r="E162" s="14"/>
-      <c r="F162" s="26"/>
+      <c r="F162" s="25"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="18"/>
@@ -3284,7 +3284,7 @@
         <v>59</v>
       </c>
       <c r="E163" s="14"/>
-      <c r="F163" s="26"/>
+      <c r="F163" s="25"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="18"/>
@@ -3296,13 +3296,13 @@
         <v>60</v>
       </c>
       <c r="E164" s="14"/>
-      <c r="F164" s="26"/>
+      <c r="F164" s="25"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="22" t="s">
+      <c r="A165" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B165" s="22" t="s">
+      <c r="B165" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C165" s="3">
@@ -3312,7 +3312,7 @@
         <v>44</v>
       </c>
       <c r="E165" s="11"/>
-      <c r="F165" s="23" t="s">
+      <c r="F165" s="26" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3326,7 +3326,7 @@
         <v>4</v>
       </c>
       <c r="E166" s="11"/>
-      <c r="F166" s="24"/>
+      <c r="F166" s="23"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="21"/>
@@ -3338,7 +3338,7 @@
         <v>57</v>
       </c>
       <c r="E167" s="11"/>
-      <c r="F167" s="24"/>
+      <c r="F167" s="23"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="21"/>
@@ -3350,7 +3350,7 @@
         <v>58</v>
       </c>
       <c r="E168" s="11"/>
-      <c r="F168" s="24"/>
+      <c r="F168" s="23"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="21"/>
@@ -3362,7 +3362,7 @@
         <v>59</v>
       </c>
       <c r="E169" s="11"/>
-      <c r="F169" s="24"/>
+      <c r="F169" s="23"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="21"/>
@@ -3374,7 +3374,7 @@
         <v>60</v>
       </c>
       <c r="E170" s="11"/>
-      <c r="F170" s="24"/>
+      <c r="F170" s="23"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="17" t="s">
@@ -3390,7 +3390,7 @@
         <v>44</v>
       </c>
       <c r="E171" s="14"/>
-      <c r="F171" s="25" t="s">
+      <c r="F171" s="24" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3404,7 +3404,7 @@
         <v>4</v>
       </c>
       <c r="E172" s="14"/>
-      <c r="F172" s="26"/>
+      <c r="F172" s="25"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="18"/>
@@ -3416,7 +3416,7 @@
         <v>57</v>
       </c>
       <c r="E173" s="14"/>
-      <c r="F173" s="26"/>
+      <c r="F173" s="25"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="18"/>
@@ -3428,7 +3428,7 @@
         <v>58</v>
       </c>
       <c r="E174" s="14"/>
-      <c r="F174" s="26"/>
+      <c r="F174" s="25"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="18"/>
@@ -3440,7 +3440,7 @@
         <v>59</v>
       </c>
       <c r="E175" s="14"/>
-      <c r="F175" s="26"/>
+      <c r="F175" s="25"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="18"/>
@@ -3452,13 +3452,13 @@
         <v>60</v>
       </c>
       <c r="E176" s="14"/>
-      <c r="F176" s="26"/>
+      <c r="F176" s="25"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="22" t="s">
+      <c r="A177" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B177" s="22" t="s">
+      <c r="B177" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C177" s="3">
@@ -3468,7 +3468,7 @@
         <v>44</v>
       </c>
       <c r="E177" s="11"/>
-      <c r="F177" s="23" t="s">
+      <c r="F177" s="26" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3482,7 +3482,7 @@
         <v>4</v>
       </c>
       <c r="E178" s="11"/>
-      <c r="F178" s="24"/>
+      <c r="F178" s="23"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="21"/>
@@ -3494,7 +3494,7 @@
         <v>57</v>
       </c>
       <c r="E179" s="11"/>
-      <c r="F179" s="24"/>
+      <c r="F179" s="23"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="21"/>
@@ -3506,7 +3506,7 @@
         <v>58</v>
       </c>
       <c r="E180" s="11"/>
-      <c r="F180" s="24"/>
+      <c r="F180" s="23"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="21"/>
@@ -3518,7 +3518,7 @@
         <v>59</v>
       </c>
       <c r="E181" s="11"/>
-      <c r="F181" s="24"/>
+      <c r="F181" s="23"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="21"/>
@@ -3530,7 +3530,7 @@
         <v>60</v>
       </c>
       <c r="E182" s="11"/>
-      <c r="F182" s="24"/>
+      <c r="F182" s="23"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
@@ -3546,7 +3546,7 @@
         <v>44</v>
       </c>
       <c r="E183" s="14"/>
-      <c r="F183" s="25" t="s">
+      <c r="F183" s="24" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3560,7 +3560,7 @@
         <v>4</v>
       </c>
       <c r="E184" s="14"/>
-      <c r="F184" s="26"/>
+      <c r="F184" s="25"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="18"/>
@@ -3572,7 +3572,7 @@
         <v>57</v>
       </c>
       <c r="E185" s="14"/>
-      <c r="F185" s="26"/>
+      <c r="F185" s="25"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="18"/>
@@ -3584,7 +3584,7 @@
         <v>58</v>
       </c>
       <c r="E186" s="14"/>
-      <c r="F186" s="26"/>
+      <c r="F186" s="25"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="18"/>
@@ -3596,7 +3596,7 @@
         <v>59</v>
       </c>
       <c r="E187" s="14"/>
-      <c r="F187" s="26"/>
+      <c r="F187" s="25"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="18"/>
@@ -3608,13 +3608,13 @@
         <v>60</v>
       </c>
       <c r="E188" s="14"/>
-      <c r="F188" s="26"/>
+      <c r="F188" s="25"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="22" t="s">
+      <c r="A189" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B189" s="22" t="s">
+      <c r="B189" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C189" s="3">
@@ -3624,7 +3624,7 @@
         <v>44</v>
       </c>
       <c r="E189" s="11"/>
-      <c r="F189" s="23" t="s">
+      <c r="F189" s="26" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3638,7 +3638,7 @@
         <v>4</v>
       </c>
       <c r="E190" s="11"/>
-      <c r="F190" s="24"/>
+      <c r="F190" s="23"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="21"/>
@@ -3650,7 +3650,7 @@
         <v>57</v>
       </c>
       <c r="E191" s="11"/>
-      <c r="F191" s="24"/>
+      <c r="F191" s="23"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="21"/>
@@ -3662,7 +3662,7 @@
         <v>58</v>
       </c>
       <c r="E192" s="11"/>
-      <c r="F192" s="24"/>
+      <c r="F192" s="23"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="21"/>
@@ -3674,7 +3674,7 @@
         <v>59</v>
       </c>
       <c r="E193" s="11"/>
-      <c r="F193" s="24"/>
+      <c r="F193" s="23"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="21"/>
@@ -3686,7 +3686,7 @@
         <v>60</v>
       </c>
       <c r="E194" s="11"/>
-      <c r="F194" s="24"/>
+      <c r="F194" s="23"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
@@ -3702,7 +3702,7 @@
         <v>44</v>
       </c>
       <c r="E195" s="14"/>
-      <c r="F195" s="25" t="s">
+      <c r="F195" s="24" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
         <v>4</v>
       </c>
       <c r="E196" s="14"/>
-      <c r="F196" s="26"/>
+      <c r="F196" s="25"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="18"/>
@@ -3728,7 +3728,7 @@
         <v>57</v>
       </c>
       <c r="E197" s="14"/>
-      <c r="F197" s="26"/>
+      <c r="F197" s="25"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="18"/>
@@ -3740,7 +3740,7 @@
         <v>58</v>
       </c>
       <c r="E198" s="14"/>
-      <c r="F198" s="26"/>
+      <c r="F198" s="25"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="18"/>
@@ -3752,7 +3752,7 @@
         <v>59</v>
       </c>
       <c r="E199" s="14"/>
-      <c r="F199" s="26"/>
+      <c r="F199" s="25"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="18"/>
@@ -3764,13 +3764,13 @@
         <v>60</v>
       </c>
       <c r="E200" s="14"/>
-      <c r="F200" s="26"/>
+      <c r="F200" s="25"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="22" t="s">
+      <c r="A201" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B201" s="22" t="s">
+      <c r="B201" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C201" s="3">
@@ -3780,13 +3780,13 @@
         <v>44</v>
       </c>
       <c r="E201" s="11"/>
-      <c r="F201" s="23" t="s">
+      <c r="F201" s="26" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="21"/>
-      <c r="B202" s="22"/>
+      <c r="B202" s="20"/>
       <c r="C202" s="3">
         <v>2</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>4</v>
       </c>
       <c r="E202" s="11"/>
-      <c r="F202" s="23"/>
+      <c r="F202" s="26"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C203"/>
@@ -3810,11 +3810,77 @@
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A73:A80"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A81:F81"/>
-    <mergeCell ref="A82:A91"/>
-    <mergeCell ref="B82:B91"/>
+    <mergeCell ref="A201:A202"/>
+    <mergeCell ref="B201:B202"/>
+    <mergeCell ref="F201:F202"/>
+    <mergeCell ref="A189:A194"/>
+    <mergeCell ref="B189:B194"/>
+    <mergeCell ref="F189:F194"/>
+    <mergeCell ref="A195:A200"/>
+    <mergeCell ref="B195:B200"/>
+    <mergeCell ref="F195:F200"/>
+    <mergeCell ref="F183:F188"/>
+    <mergeCell ref="A165:A170"/>
+    <mergeCell ref="B165:B170"/>
+    <mergeCell ref="F165:F170"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="B171:B176"/>
+    <mergeCell ref="F171:F176"/>
+    <mergeCell ref="A177:A182"/>
+    <mergeCell ref="B177:B182"/>
+    <mergeCell ref="F177:F182"/>
+    <mergeCell ref="A183:A188"/>
+    <mergeCell ref="B183:B188"/>
+    <mergeCell ref="A153:A158"/>
+    <mergeCell ref="B153:B158"/>
+    <mergeCell ref="F153:F158"/>
+    <mergeCell ref="A159:A164"/>
+    <mergeCell ref="B159:B164"/>
+    <mergeCell ref="F159:F164"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="B147:B152"/>
+    <mergeCell ref="F147:F152"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="F132:F136"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="F137:F141"/>
+    <mergeCell ref="A121:F121"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="F122:F126"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="F127:F131"/>
+    <mergeCell ref="A110:A114"/>
+    <mergeCell ref="B110:B114"/>
+    <mergeCell ref="F110:F114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="F115:F120"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="F105:F109"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="B105:B109"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="B92:B101"/>
     <mergeCell ref="A92:A101"/>
     <mergeCell ref="A2:F2"/>
@@ -3831,81 +3897,15 @@
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B18"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A73:A80"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="A82:A91"/>
+    <mergeCell ref="B82:B91"/>
     <mergeCell ref="B69:B72"/>
     <mergeCell ref="A69:A72"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="F105:F109"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="B105:B109"/>
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="B110:B114"/>
-    <mergeCell ref="F110:F114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="B115:B120"/>
-    <mergeCell ref="F115:F120"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A122:A126"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="F122:F126"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="F127:F131"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="F132:F136"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="F137:F141"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="F142:F146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="B147:B152"/>
-    <mergeCell ref="F147:F152"/>
-    <mergeCell ref="A153:A158"/>
-    <mergeCell ref="B153:B158"/>
-    <mergeCell ref="F153:F158"/>
-    <mergeCell ref="A159:A164"/>
-    <mergeCell ref="B159:B164"/>
-    <mergeCell ref="F159:F164"/>
-    <mergeCell ref="F183:F188"/>
-    <mergeCell ref="A165:A170"/>
-    <mergeCell ref="B165:B170"/>
-    <mergeCell ref="F165:F170"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="B171:B176"/>
-    <mergeCell ref="F171:F176"/>
     <mergeCell ref="B73:B80"/>
     <mergeCell ref="F73:F80"/>
-    <mergeCell ref="A201:A202"/>
-    <mergeCell ref="B201:B202"/>
-    <mergeCell ref="F201:F202"/>
-    <mergeCell ref="A189:A194"/>
-    <mergeCell ref="B189:B194"/>
-    <mergeCell ref="F189:F194"/>
-    <mergeCell ref="A195:A200"/>
-    <mergeCell ref="B195:B200"/>
-    <mergeCell ref="F195:F200"/>
-    <mergeCell ref="A177:A182"/>
-    <mergeCell ref="B177:B182"/>
-    <mergeCell ref="F177:F182"/>
-    <mergeCell ref="A183:A188"/>
-    <mergeCell ref="B183:B188"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Discovered mistake in 10-pos Microclasp pinout diagram
</commit_message>
<xml_diff>
--- a/MCN Breakout Pinouts.xlsx
+++ b/MCN Breakout Pinouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="12375"/>
@@ -499,22 +499,31 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,17 +532,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116:B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,20 +879,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="3">
@@ -909,8 +909,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -925,8 +925,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3">
         <v>3</v>
       </c>
@@ -941,8 +941,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3">
         <v>4</v>
       </c>
@@ -957,8 +957,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="3">
         <v>5</v>
       </c>
@@ -969,8 +969,8 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3">
         <v>6</v>
       </c>
@@ -985,8 +985,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="3">
         <v>7</v>
       </c>
@@ -1001,8 +1001,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="3">
         <v>8</v>
       </c>
@@ -1013,10 +1013,10 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="5">
@@ -1033,8 +1033,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5">
         <v>2</v>
       </c>
@@ -1049,8 +1049,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5">
         <v>3</v>
       </c>
@@ -1065,8 +1065,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -1081,8 +1081,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5">
         <v>5</v>
       </c>
@@ -1097,8 +1097,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5">
         <v>6</v>
       </c>
@@ -1113,8 +1113,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="5">
         <v>7</v>
       </c>
@@ -1129,8 +1129,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5">
         <v>8</v>
       </c>
@@ -1145,10 +1145,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="3">
@@ -1165,8 +1165,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="3">
         <v>2</v>
       </c>
@@ -1177,8 +1177,8 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="3">
         <v>3</v>
       </c>
@@ -1193,8 +1193,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="3">
         <v>4</v>
       </c>
@@ -1209,8 +1209,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="3">
         <v>5</v>
       </c>
@@ -1221,8 +1221,8 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="3">
         <v>6</v>
       </c>
@@ -1237,8 +1237,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="3">
         <v>7</v>
       </c>
@@ -1253,8 +1253,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="3">
         <v>8</v>
       </c>
@@ -1265,10 +1265,10 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="5">
@@ -1285,8 +1285,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="5">
         <v>2</v>
       </c>
@@ -1301,8 +1301,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="5">
         <v>3</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="5">
         <v>4</v>
       </c>
@@ -1329,20 +1329,20 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="3">
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="3">
         <v>2</v>
       </c>
@@ -1375,8 +1375,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="3">
         <v>3</v>
       </c>
@@ -1391,8 +1391,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="3">
         <v>4</v>
       </c>
@@ -1407,8 +1407,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="3">
         <v>5</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="3">
         <v>6</v>
       </c>
@@ -1439,8 +1439,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
       <c r="C38" s="3">
         <v>7</v>
       </c>
@@ -1455,8 +1455,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
       <c r="C39" s="3">
         <v>8</v>
       </c>
@@ -1467,10 +1467,10 @@
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="5">
@@ -1487,8 +1487,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="5">
         <v>2</v>
       </c>
@@ -1503,8 +1503,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="5">
         <v>3</v>
       </c>
@@ -1519,8 +1519,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="5">
         <v>4</v>
       </c>
@@ -1535,8 +1535,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="5">
         <v>5</v>
       </c>
@@ -1551,8 +1551,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="5">
         <v>6</v>
       </c>
@@ -1567,8 +1567,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="5">
         <v>7</v>
       </c>
@@ -1583,8 +1583,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="5">
         <v>8</v>
       </c>
@@ -1599,10 +1599,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="3">
@@ -1619,8 +1619,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="3">
         <v>2</v>
       </c>
@@ -1635,8 +1635,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="3">
         <v>3</v>
       </c>
@@ -1651,8 +1651,8 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="3">
         <v>4</v>
       </c>
@@ -1667,8 +1667,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
       <c r="C52" s="3">
         <v>5</v>
       </c>
@@ -1683,8 +1683,8 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="3">
         <v>6</v>
       </c>
@@ -1695,8 +1695,8 @@
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
       <c r="C54" s="3">
         <v>7</v>
       </c>
@@ -1707,8 +1707,8 @@
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
       <c r="C55" s="3">
         <v>8</v>
       </c>
@@ -1719,10 +1719,10 @@
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C56" s="5">
@@ -1739,8 +1739,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
       <c r="C57" s="5">
         <v>2</v>
       </c>
@@ -1755,8 +1755,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
       <c r="C58" s="5">
         <v>3</v>
       </c>
@@ -1771,8 +1771,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
       <c r="C59" s="5">
         <v>4</v>
       </c>
@@ -1787,8 +1787,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
       <c r="C60" s="5">
         <v>5</v>
       </c>
@@ -1803,8 +1803,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
       <c r="C61" s="5">
         <v>6</v>
       </c>
@@ -1815,8 +1815,8 @@
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
       <c r="C62" s="5">
         <v>7</v>
       </c>
@@ -1827,8 +1827,8 @@
       <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
       <c r="C63" s="5">
         <v>8</v>
       </c>
@@ -1839,20 +1839,20 @@
       <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C65" s="3">
@@ -1869,8 +1869,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
       <c r="C66" s="3">
         <v>2</v>
       </c>
@@ -1885,8 +1885,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
       <c r="C67" s="3">
         <v>3</v>
       </c>
@@ -1901,8 +1901,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
       <c r="C68" s="3">
         <v>4</v>
       </c>
@@ -1913,8 +1913,8 @@
       <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
       <c r="C69" s="3">
         <v>5</v>
       </c>
@@ -1925,8 +1925,8 @@
       <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
       <c r="C70" s="3">
         <v>6</v>
       </c>
@@ -1937,8 +1937,8 @@
       <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
       <c r="C71" s="3">
         <v>7</v>
       </c>
@@ -1949,8 +1949,8 @@
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
       <c r="C72" s="3">
         <v>8</v>
       </c>
@@ -1961,10 +1961,10 @@
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C73" s="5">
@@ -1981,8 +1981,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
-      <c r="B74" s="22"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
       <c r="C74" s="5">
         <v>2</v>
       </c>
@@ -1997,8 +1997,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
       <c r="C75" s="5">
         <v>3</v>
       </c>
@@ -2013,8 +2013,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
       <c r="C76" s="5">
         <v>4</v>
       </c>
@@ -2025,8 +2025,8 @@
       <c r="F76" s="6"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
       <c r="C77" s="5">
         <v>5</v>
       </c>
@@ -2037,8 +2037,8 @@
       <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" s="22"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="5">
         <v>6</v>
       </c>
@@ -2049,8 +2049,8 @@
       <c r="F78" s="6"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="22"/>
-      <c r="B79" s="22"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
       <c r="C79" s="5">
         <v>7</v>
       </c>
@@ -2061,8 +2061,8 @@
       <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="22"/>
-      <c r="B80" s="22"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
       <c r="C80" s="5">
         <v>8</v>
       </c>
@@ -2073,10 +2073,10 @@
       <c r="F80" s="6"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C81" s="3">
@@ -2093,8 +2093,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
       <c r="C82" s="3">
         <v>2</v>
       </c>
@@ -2109,8 +2109,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
-      <c r="B83" s="18"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
       <c r="C83" s="3">
         <v>3</v>
       </c>
@@ -2125,8 +2125,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
-      <c r="B84" s="18"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
       <c r="C84" s="3">
         <v>4</v>
       </c>
@@ -2137,8 +2137,8 @@
       <c r="F84" s="4"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="3">
         <v>5</v>
       </c>
@@ -2149,8 +2149,8 @@
       <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
-      <c r="B86" s="18"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
       <c r="C86" s="3">
         <v>6</v>
       </c>
@@ -2161,8 +2161,8 @@
       <c r="F86" s="4"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
-      <c r="B87" s="18"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
       <c r="C87" s="3">
         <v>7</v>
       </c>
@@ -2173,8 +2173,8 @@
       <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="18"/>
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
       <c r="C88" s="3">
         <v>8</v>
       </c>
@@ -2185,10 +2185,10 @@
       <c r="F88" s="4"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C89" s="5">
@@ -2205,8 +2205,8 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="22"/>
-      <c r="B90" s="21"/>
+      <c r="A90" s="18"/>
+      <c r="B90" s="17"/>
       <c r="C90" s="5">
         <v>2</v>
       </c>
@@ -2221,8 +2221,8 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="22"/>
-      <c r="B91" s="21"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="17"/>
       <c r="C91" s="5">
         <v>3</v>
       </c>
@@ -2237,8 +2237,8 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="22"/>
-      <c r="B92" s="21"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="17"/>
       <c r="C92" s="5">
         <v>4</v>
       </c>
@@ -2253,10 +2253,10 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C93" s="3">
@@ -2273,8 +2273,8 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="18"/>
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
       <c r="C94" s="3">
         <v>2</v>
       </c>
@@ -2289,8 +2289,8 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="18"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="21"/>
       <c r="C95" s="3">
         <v>3</v>
       </c>
@@ -2305,8 +2305,8 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
-      <c r="B96" s="18"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
       <c r="C96" s="3">
         <v>4</v>
       </c>
@@ -2321,10 +2321,10 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="21" t="s">
+      <c r="A97" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B97" s="21" t="s">
+      <c r="B97" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C97" s="5">
@@ -2336,13 +2336,13 @@
       <c r="E97" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F97" s="27" t="s">
+      <c r="F97" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="22"/>
-      <c r="B98" s="22"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="18"/>
       <c r="C98" s="5">
         <v>2</v>
       </c>
@@ -2352,11 +2352,11 @@
       <c r="E98" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F98" s="28"/>
+      <c r="F98" s="23"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="22"/>
-      <c r="B99" s="22"/>
+      <c r="A99" s="18"/>
+      <c r="B99" s="18"/>
       <c r="C99" s="5">
         <v>3</v>
       </c>
@@ -2366,11 +2366,11 @@
       <c r="E99" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F99" s="28"/>
+      <c r="F99" s="23"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="22"/>
-      <c r="B100" s="22"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="18"/>
       <c r="C100" s="5">
         <v>4</v>
       </c>
@@ -2380,11 +2380,11 @@
       <c r="E100" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F100" s="28"/>
+      <c r="F100" s="23"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="22"/>
-      <c r="B101" s="22"/>
+      <c r="A101" s="18"/>
+      <c r="B101" s="18"/>
       <c r="C101" s="5">
         <v>5</v>
       </c>
@@ -2394,11 +2394,11 @@
       <c r="E101" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F101" s="28"/>
+      <c r="F101" s="23"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
-      <c r="B102" s="22"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
       <c r="C102" s="5">
         <v>6</v>
       </c>
@@ -2408,11 +2408,11 @@
       <c r="E102" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F102" s="28"/>
+      <c r="F102" s="23"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="22"/>
-      <c r="B103" s="22"/>
+      <c r="A103" s="18"/>
+      <c r="B103" s="18"/>
       <c r="C103" s="5">
         <v>7</v>
       </c>
@@ -2422,11 +2422,11 @@
       <c r="E103" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F103" s="28"/>
+      <c r="F103" s="23"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="22"/>
-      <c r="B104" s="22"/>
+      <c r="A104" s="18"/>
+      <c r="B104" s="18"/>
       <c r="C104" s="5">
         <v>8</v>
       </c>
@@ -2436,23 +2436,23 @@
       <c r="E104" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F104" s="28"/>
+      <c r="F104" s="23"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="25" t="s">
+      <c r="A105" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="20" t="s">
         <v>95</v>
       </c>
       <c r="C106" s="3">
@@ -2469,8 +2469,8 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="18"/>
-      <c r="B107" s="18"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="21"/>
       <c r="C107" s="3">
         <v>2</v>
       </c>
@@ -2485,8 +2485,8 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="18"/>
-      <c r="B108" s="18"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
       <c r="C108" s="3">
         <v>3</v>
       </c>
@@ -2501,8 +2501,8 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="18"/>
-      <c r="B109" s="18"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="21"/>
       <c r="C109" s="3">
         <v>4</v>
       </c>
@@ -2517,8 +2517,8 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="18"/>
-      <c r="B110" s="18"/>
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
       <c r="C110" s="3">
         <v>5</v>
       </c>
@@ -2533,8 +2533,8 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="18"/>
-      <c r="B111" s="18"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
       <c r="C111" s="3">
         <v>6</v>
       </c>
@@ -2549,8 +2549,8 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="18"/>
-      <c r="B112" s="18"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
       <c r="C112" s="3">
         <v>7</v>
       </c>
@@ -2565,8 +2565,8 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="18"/>
-      <c r="B113" s="18"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
       <c r="C113" s="3">
         <v>8</v>
       </c>
@@ -2581,8 +2581,8 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="18"/>
-      <c r="B114" s="18"/>
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
       <c r="C114" s="3">
         <v>9</v>
       </c>
@@ -2597,8 +2597,8 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="18"/>
-      <c r="B115" s="18"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
       <c r="C115" s="3">
         <v>10</v>
       </c>
@@ -2609,10 +2609,10 @@
       <c r="F115" s="4"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="21" t="s">
+      <c r="A116" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B116" s="22" t="s">
+      <c r="B116" s="18" t="s">
         <v>95</v>
       </c>
       <c r="C116" s="5">
@@ -2629,8 +2629,8 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="21"/>
-      <c r="B117" s="22"/>
+      <c r="A117" s="17"/>
+      <c r="B117" s="18"/>
       <c r="C117" s="5">
         <v>2</v>
       </c>
@@ -2645,8 +2645,8 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="21"/>
-      <c r="B118" s="22"/>
+      <c r="A118" s="17"/>
+      <c r="B118" s="18"/>
       <c r="C118" s="5">
         <v>3</v>
       </c>
@@ -2661,8 +2661,8 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="21"/>
-      <c r="B119" s="22"/>
+      <c r="A119" s="17"/>
+      <c r="B119" s="18"/>
       <c r="C119" s="5">
         <v>4</v>
       </c>
@@ -2677,8 +2677,8 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="21"/>
-      <c r="B120" s="22"/>
+      <c r="A120" s="17"/>
+      <c r="B120" s="18"/>
       <c r="C120" s="5">
         <v>5</v>
       </c>
@@ -2693,24 +2693,20 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="21"/>
-      <c r="B121" s="22"/>
+      <c r="A121" s="17"/>
+      <c r="B121" s="18"/>
       <c r="C121" s="5">
         <v>6</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E121" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F121" s="7" t="s">
-        <v>98</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E121" s="13"/>
+      <c r="F121" s="6"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="21"/>
-      <c r="B122" s="22"/>
+      <c r="A122" s="17"/>
+      <c r="B122" s="18"/>
       <c r="C122" s="5">
         <v>7</v>
       </c>
@@ -2721,8 +2717,8 @@
       <c r="F122" s="6"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="21"/>
-      <c r="B123" s="22"/>
+      <c r="A123" s="17"/>
+      <c r="B123" s="18"/>
       <c r="C123" s="5">
         <v>8</v>
       </c>
@@ -2733,8 +2729,8 @@
       <c r="F123" s="6"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="21"/>
-      <c r="B124" s="22"/>
+      <c r="A124" s="17"/>
+      <c r="B124" s="18"/>
       <c r="C124" s="5">
         <v>9</v>
       </c>
@@ -2745,32 +2741,36 @@
       <c r="F124" s="6"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="21"/>
-      <c r="B125" s="22"/>
+      <c r="A125" s="17"/>
+      <c r="B125" s="18"/>
       <c r="C125" s="5">
         <v>10</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E125" s="13"/>
-      <c r="F125" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="25" t="s">
+      <c r="A126" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B126" s="25"/>
-      <c r="C126" s="25"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="25"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="19"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="19"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="17" t="s">
+      <c r="A127" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C127" s="3">
@@ -2780,13 +2780,13 @@
         <v>42</v>
       </c>
       <c r="E127" s="15"/>
-      <c r="F127" s="20" t="s">
+      <c r="F127" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="18"/>
-      <c r="B128" s="18"/>
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
       <c r="C128" s="3">
         <v>2</v>
       </c>
@@ -2794,13 +2794,13 @@
         <v>4</v>
       </c>
       <c r="E128" s="15"/>
-      <c r="F128" s="20"/>
+      <c r="F128" s="25"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="21" t="s">
+      <c r="A129" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C129" s="5">
@@ -2810,13 +2810,13 @@
         <v>55</v>
       </c>
       <c r="E129" s="14"/>
-      <c r="F129" s="23" t="s">
+      <c r="F129" s="26" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="22"/>
-      <c r="B130" s="22"/>
+      <c r="A130" s="18"/>
+      <c r="B130" s="18"/>
       <c r="C130" s="5">
         <v>2</v>
       </c>
@@ -2824,11 +2824,11 @@
         <v>42</v>
       </c>
       <c r="E130" s="14"/>
-      <c r="F130" s="24"/>
+      <c r="F130" s="27"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="22"/>
-      <c r="B131" s="22"/>
+      <c r="A131" s="18"/>
+      <c r="B131" s="18"/>
       <c r="C131" s="5">
         <v>3</v>
       </c>
@@ -2836,11 +2836,11 @@
         <v>4</v>
       </c>
       <c r="E131" s="14"/>
-      <c r="F131" s="24"/>
+      <c r="F131" s="27"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="22"/>
-      <c r="B132" s="22"/>
+      <c r="A132" s="18"/>
+      <c r="B132" s="18"/>
       <c r="C132" s="5">
         <v>4</v>
       </c>
@@ -2848,11 +2848,11 @@
         <v>56</v>
       </c>
       <c r="E132" s="14"/>
-      <c r="F132" s="24"/>
+      <c r="F132" s="27"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="22"/>
-      <c r="B133" s="22"/>
+      <c r="A133" s="18"/>
+      <c r="B133" s="18"/>
       <c r="C133" s="5">
         <v>5</v>
       </c>
@@ -2860,13 +2860,13 @@
         <v>57</v>
       </c>
       <c r="E133" s="14"/>
-      <c r="F133" s="24"/>
+      <c r="F133" s="27"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
+      <c r="A134" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C134" s="3">
@@ -2876,13 +2876,13 @@
         <v>55</v>
       </c>
       <c r="E134" s="11"/>
-      <c r="F134" s="17" t="s">
+      <c r="F134" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="18"/>
-      <c r="B135" s="18"/>
+      <c r="A135" s="21"/>
+      <c r="B135" s="21"/>
       <c r="C135" s="3">
         <v>2</v>
       </c>
@@ -2890,11 +2890,11 @@
         <v>42</v>
       </c>
       <c r="E135" s="11"/>
-      <c r="F135" s="18"/>
+      <c r="F135" s="21"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="18"/>
-      <c r="B136" s="18"/>
+      <c r="A136" s="21"/>
+      <c r="B136" s="21"/>
       <c r="C136" s="3">
         <v>3</v>
       </c>
@@ -2902,11 +2902,11 @@
         <v>4</v>
       </c>
       <c r="E136" s="11"/>
-      <c r="F136" s="18"/>
+      <c r="F136" s="21"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="18"/>
-      <c r="B137" s="18"/>
+      <c r="A137" s="21"/>
+      <c r="B137" s="21"/>
       <c r="C137" s="3">
         <v>4</v>
       </c>
@@ -2914,11 +2914,11 @@
         <v>56</v>
       </c>
       <c r="E137" s="11"/>
-      <c r="F137" s="18"/>
+      <c r="F137" s="21"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="18"/>
-      <c r="B138" s="18"/>
+      <c r="A138" s="21"/>
+      <c r="B138" s="21"/>
       <c r="C138" s="3">
         <v>5</v>
       </c>
@@ -2926,13 +2926,13 @@
         <v>57</v>
       </c>
       <c r="E138" s="11"/>
-      <c r="F138" s="18"/>
+      <c r="F138" s="21"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="21" t="s">
+      <c r="A139" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B139" s="22" t="s">
+      <c r="B139" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C139" s="5">
@@ -2942,13 +2942,13 @@
         <v>42</v>
       </c>
       <c r="E139" s="13"/>
-      <c r="F139" s="22" t="s">
+      <c r="F139" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="22"/>
-      <c r="B140" s="22"/>
+      <c r="A140" s="18"/>
+      <c r="B140" s="18"/>
       <c r="C140" s="5">
         <v>2</v>
       </c>
@@ -2956,11 +2956,11 @@
         <v>4</v>
       </c>
       <c r="E140" s="13"/>
-      <c r="F140" s="22"/>
+      <c r="F140" s="18"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="22"/>
-      <c r="B141" s="22"/>
+      <c r="A141" s="18"/>
+      <c r="B141" s="18"/>
       <c r="C141" s="5">
         <v>3</v>
       </c>
@@ -2968,11 +2968,11 @@
         <v>55</v>
       </c>
       <c r="E141" s="13"/>
-      <c r="F141" s="22"/>
+      <c r="F141" s="18"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="22"/>
-      <c r="B142" s="22"/>
+      <c r="A142" s="18"/>
+      <c r="B142" s="18"/>
       <c r="C142" s="5">
         <v>4</v>
       </c>
@@ -2980,11 +2980,11 @@
         <v>56</v>
       </c>
       <c r="E142" s="13"/>
-      <c r="F142" s="22"/>
+      <c r="F142" s="18"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="22"/>
-      <c r="B143" s="22"/>
+      <c r="A143" s="18"/>
+      <c r="B143" s="18"/>
       <c r="C143" s="5">
         <v>5</v>
       </c>
@@ -2992,11 +2992,11 @@
         <v>57</v>
       </c>
       <c r="E143" s="13"/>
-      <c r="F143" s="22"/>
+      <c r="F143" s="18"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="22"/>
-      <c r="B144" s="22"/>
+      <c r="A144" s="18"/>
+      <c r="B144" s="18"/>
       <c r="C144" s="5">
         <v>6</v>
       </c>
@@ -3004,23 +3004,23 @@
         <v>58</v>
       </c>
       <c r="E144" s="13"/>
-      <c r="F144" s="22"/>
+      <c r="F144" s="18"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="25" t="s">
+      <c r="A145" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B145" s="25"/>
-      <c r="C145" s="25"/>
-      <c r="D145" s="25"/>
-      <c r="E145" s="25"/>
-      <c r="F145" s="25"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="19"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="19"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
+      <c r="A146" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B146" s="18" t="s">
+      <c r="B146" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C146" s="3">
@@ -3030,13 +3030,13 @@
         <v>55</v>
       </c>
       <c r="E146" s="11"/>
-      <c r="F146" s="19" t="s">
+      <c r="F146" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="18"/>
-      <c r="B147" s="18"/>
+      <c r="A147" s="21"/>
+      <c r="B147" s="21"/>
       <c r="C147" s="3">
         <v>2</v>
       </c>
@@ -3044,11 +3044,11 @@
         <v>42</v>
       </c>
       <c r="E147" s="11"/>
-      <c r="F147" s="20"/>
+      <c r="F147" s="25"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="18"/>
-      <c r="B148" s="18"/>
+      <c r="A148" s="21"/>
+      <c r="B148" s="21"/>
       <c r="C148" s="3">
         <v>3</v>
       </c>
@@ -3056,11 +3056,11 @@
         <v>4</v>
       </c>
       <c r="E148" s="11"/>
-      <c r="F148" s="20"/>
+      <c r="F148" s="25"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="18"/>
-      <c r="B149" s="18"/>
+      <c r="A149" s="21"/>
+      <c r="B149" s="21"/>
       <c r="C149" s="3">
         <v>4</v>
       </c>
@@ -3068,11 +3068,11 @@
         <v>56</v>
       </c>
       <c r="E149" s="11"/>
-      <c r="F149" s="20"/>
+      <c r="F149" s="25"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="18"/>
-      <c r="B150" s="18"/>
+      <c r="A150" s="21"/>
+      <c r="B150" s="21"/>
       <c r="C150" s="3">
         <v>5</v>
       </c>
@@ -3080,13 +3080,13 @@
         <v>57</v>
       </c>
       <c r="E150" s="11"/>
-      <c r="F150" s="20"/>
+      <c r="F150" s="25"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="21" t="s">
+      <c r="A151" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B151" s="21" t="s">
+      <c r="B151" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C151" s="5">
@@ -3096,13 +3096,13 @@
         <v>55</v>
       </c>
       <c r="E151" s="14"/>
-      <c r="F151" s="23" t="s">
+      <c r="F151" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="22"/>
-      <c r="B152" s="22"/>
+      <c r="A152" s="18"/>
+      <c r="B152" s="18"/>
       <c r="C152" s="5">
         <v>2</v>
       </c>
@@ -3110,11 +3110,11 @@
         <v>42</v>
       </c>
       <c r="E152" s="14"/>
-      <c r="F152" s="24"/>
+      <c r="F152" s="27"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="22"/>
-      <c r="B153" s="22"/>
+      <c r="A153" s="18"/>
+      <c r="B153" s="18"/>
       <c r="C153" s="5">
         <v>3</v>
       </c>
@@ -3122,11 +3122,11 @@
         <v>4</v>
       </c>
       <c r="E153" s="14"/>
-      <c r="F153" s="24"/>
+      <c r="F153" s="27"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="22"/>
-      <c r="B154" s="22"/>
+      <c r="A154" s="18"/>
+      <c r="B154" s="18"/>
       <c r="C154" s="5">
         <v>4</v>
       </c>
@@ -3134,11 +3134,11 @@
         <v>56</v>
       </c>
       <c r="E154" s="14"/>
-      <c r="F154" s="24"/>
+      <c r="F154" s="27"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="22"/>
-      <c r="B155" s="22"/>
+      <c r="A155" s="18"/>
+      <c r="B155" s="18"/>
       <c r="C155" s="5">
         <v>5</v>
       </c>
@@ -3146,13 +3146,13 @@
         <v>57</v>
       </c>
       <c r="E155" s="14"/>
-      <c r="F155" s="24"/>
+      <c r="F155" s="27"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="17" t="s">
+      <c r="A156" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B156" s="18" t="s">
+      <c r="B156" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C156" s="3">
@@ -3162,13 +3162,13 @@
         <v>55</v>
       </c>
       <c r="E156" s="11"/>
-      <c r="F156" s="19" t="s">
+      <c r="F156" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="18"/>
-      <c r="B157" s="18"/>
+      <c r="A157" s="21"/>
+      <c r="B157" s="21"/>
       <c r="C157" s="3">
         <v>2</v>
       </c>
@@ -3176,11 +3176,11 @@
         <v>42</v>
       </c>
       <c r="E157" s="11"/>
-      <c r="F157" s="20"/>
+      <c r="F157" s="25"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="18"/>
-      <c r="B158" s="18"/>
+      <c r="A158" s="21"/>
+      <c r="B158" s="21"/>
       <c r="C158" s="3">
         <v>3</v>
       </c>
@@ -3188,11 +3188,11 @@
         <v>4</v>
       </c>
       <c r="E158" s="11"/>
-      <c r="F158" s="20"/>
+      <c r="F158" s="25"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="18"/>
-      <c r="B159" s="18"/>
+      <c r="A159" s="21"/>
+      <c r="B159" s="21"/>
       <c r="C159" s="3">
         <v>4</v>
       </c>
@@ -3200,11 +3200,11 @@
         <v>56</v>
       </c>
       <c r="E159" s="11"/>
-      <c r="F159" s="20"/>
+      <c r="F159" s="25"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="18"/>
-      <c r="B160" s="18"/>
+      <c r="A160" s="21"/>
+      <c r="B160" s="21"/>
       <c r="C160" s="3">
         <v>5</v>
       </c>
@@ -3212,13 +3212,13 @@
         <v>57</v>
       </c>
       <c r="E160" s="11"/>
-      <c r="F160" s="20"/>
+      <c r="F160" s="25"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="21" t="s">
+      <c r="A161" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B161" s="21" t="s">
+      <c r="B161" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C161" s="5">
@@ -3228,13 +3228,13 @@
         <v>55</v>
       </c>
       <c r="E161" s="14"/>
-      <c r="F161" s="23" t="s">
+      <c r="F161" s="26" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="22"/>
-      <c r="B162" s="22"/>
+      <c r="A162" s="18"/>
+      <c r="B162" s="18"/>
       <c r="C162" s="5">
         <v>2</v>
       </c>
@@ -3242,11 +3242,11 @@
         <v>42</v>
       </c>
       <c r="E162" s="14"/>
-      <c r="F162" s="24"/>
+      <c r="F162" s="27"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="22"/>
-      <c r="B163" s="22"/>
+      <c r="A163" s="18"/>
+      <c r="B163" s="18"/>
       <c r="C163" s="5">
         <v>3</v>
       </c>
@@ -3254,11 +3254,11 @@
         <v>4</v>
       </c>
       <c r="E163" s="14"/>
-      <c r="F163" s="24"/>
+      <c r="F163" s="27"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="22"/>
-      <c r="B164" s="22"/>
+      <c r="A164" s="18"/>
+      <c r="B164" s="18"/>
       <c r="C164" s="5">
         <v>4</v>
       </c>
@@ -3266,11 +3266,11 @@
         <v>56</v>
       </c>
       <c r="E164" s="14"/>
-      <c r="F164" s="24"/>
+      <c r="F164" s="27"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="22"/>
-      <c r="B165" s="22"/>
+      <c r="A165" s="18"/>
+      <c r="B165" s="18"/>
       <c r="C165" s="5">
         <v>5</v>
       </c>
@@ -3278,13 +3278,13 @@
         <v>57</v>
       </c>
       <c r="E165" s="14"/>
-      <c r="F165" s="24"/>
+      <c r="F165" s="27"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="17" t="s">
+      <c r="A166" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B166" s="18" t="s">
+      <c r="B166" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C166" s="3">
@@ -3294,13 +3294,13 @@
         <v>55</v>
       </c>
       <c r="E166" s="11"/>
-      <c r="F166" s="19" t="s">
+      <c r="F166" s="28" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="18"/>
-      <c r="B167" s="18"/>
+      <c r="A167" s="21"/>
+      <c r="B167" s="21"/>
       <c r="C167" s="3">
         <v>2</v>
       </c>
@@ -3308,11 +3308,11 @@
         <v>42</v>
       </c>
       <c r="E167" s="11"/>
-      <c r="F167" s="20"/>
+      <c r="F167" s="25"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="18"/>
-      <c r="B168" s="18"/>
+      <c r="A168" s="21"/>
+      <c r="B168" s="21"/>
       <c r="C168" s="3">
         <v>3</v>
       </c>
@@ -3320,11 +3320,11 @@
         <v>4</v>
       </c>
       <c r="E168" s="11"/>
-      <c r="F168" s="20"/>
+      <c r="F168" s="25"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="18"/>
-      <c r="B169" s="18"/>
+      <c r="A169" s="21"/>
+      <c r="B169" s="21"/>
       <c r="C169" s="3">
         <v>4</v>
       </c>
@@ -3332,11 +3332,11 @@
         <v>56</v>
       </c>
       <c r="E169" s="11"/>
-      <c r="F169" s="20"/>
+      <c r="F169" s="25"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="18"/>
-      <c r="B170" s="18"/>
+      <c r="A170" s="21"/>
+      <c r="B170" s="21"/>
       <c r="C170" s="3">
         <v>5</v>
       </c>
@@ -3344,13 +3344,13 @@
         <v>57</v>
       </c>
       <c r="E170" s="11"/>
-      <c r="F170" s="20"/>
+      <c r="F170" s="25"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="21" t="s">
+      <c r="A171" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B171" s="21" t="s">
+      <c r="B171" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C171" s="5">
@@ -3360,13 +3360,13 @@
         <v>42</v>
       </c>
       <c r="E171" s="14"/>
-      <c r="F171" s="23" t="s">
+      <c r="F171" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="22"/>
-      <c r="B172" s="22"/>
+      <c r="A172" s="18"/>
+      <c r="B172" s="18"/>
       <c r="C172" s="5">
         <v>2</v>
       </c>
@@ -3374,11 +3374,11 @@
         <v>4</v>
       </c>
       <c r="E172" s="14"/>
-      <c r="F172" s="24"/>
+      <c r="F172" s="27"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="22"/>
-      <c r="B173" s="22"/>
+      <c r="A173" s="18"/>
+      <c r="B173" s="18"/>
       <c r="C173" s="5">
         <v>3</v>
       </c>
@@ -3386,11 +3386,11 @@
         <v>55</v>
       </c>
       <c r="E173" s="14"/>
-      <c r="F173" s="24"/>
+      <c r="F173" s="27"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="22"/>
-      <c r="B174" s="22"/>
+      <c r="A174" s="18"/>
+      <c r="B174" s="18"/>
       <c r="C174" s="5">
         <v>4</v>
       </c>
@@ -3398,11 +3398,11 @@
         <v>56</v>
       </c>
       <c r="E174" s="14"/>
-      <c r="F174" s="24"/>
+      <c r="F174" s="27"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="22"/>
-      <c r="B175" s="22"/>
+      <c r="A175" s="18"/>
+      <c r="B175" s="18"/>
       <c r="C175" s="5">
         <v>5</v>
       </c>
@@ -3410,11 +3410,11 @@
         <v>57</v>
       </c>
       <c r="E175" s="14"/>
-      <c r="F175" s="24"/>
+      <c r="F175" s="27"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="22"/>
-      <c r="B176" s="22"/>
+      <c r="A176" s="18"/>
+      <c r="B176" s="18"/>
       <c r="C176" s="5">
         <v>6</v>
       </c>
@@ -3422,13 +3422,13 @@
         <v>58</v>
       </c>
       <c r="E176" s="14"/>
-      <c r="F176" s="24"/>
+      <c r="F176" s="27"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="17" t="s">
+      <c r="A177" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B177" s="17" t="s">
+      <c r="B177" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C177" s="3">
@@ -3438,13 +3438,13 @@
         <v>42</v>
       </c>
       <c r="E177" s="11"/>
-      <c r="F177" s="19" t="s">
+      <c r="F177" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="18"/>
-      <c r="B178" s="18"/>
+      <c r="A178" s="21"/>
+      <c r="B178" s="21"/>
       <c r="C178" s="3">
         <v>2</v>
       </c>
@@ -3452,11 +3452,11 @@
         <v>4</v>
       </c>
       <c r="E178" s="11"/>
-      <c r="F178" s="20"/>
+      <c r="F178" s="25"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" s="18"/>
-      <c r="B179" s="18"/>
+      <c r="A179" s="21"/>
+      <c r="B179" s="21"/>
       <c r="C179" s="3">
         <v>3</v>
       </c>
@@ -3464,11 +3464,11 @@
         <v>55</v>
       </c>
       <c r="E179" s="11"/>
-      <c r="F179" s="20"/>
+      <c r="F179" s="25"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="18"/>
-      <c r="B180" s="18"/>
+      <c r="A180" s="21"/>
+      <c r="B180" s="21"/>
       <c r="C180" s="3">
         <v>4</v>
       </c>
@@ -3476,11 +3476,11 @@
         <v>56</v>
       </c>
       <c r="E180" s="11"/>
-      <c r="F180" s="20"/>
+      <c r="F180" s="25"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="18"/>
-      <c r="B181" s="18"/>
+      <c r="A181" s="21"/>
+      <c r="B181" s="21"/>
       <c r="C181" s="3">
         <v>5</v>
       </c>
@@ -3488,11 +3488,11 @@
         <v>57</v>
       </c>
       <c r="E181" s="11"/>
-      <c r="F181" s="20"/>
+      <c r="F181" s="25"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="18"/>
-      <c r="B182" s="18"/>
+      <c r="A182" s="21"/>
+      <c r="B182" s="21"/>
       <c r="C182" s="3">
         <v>6</v>
       </c>
@@ -3500,13 +3500,13 @@
         <v>58</v>
       </c>
       <c r="E182" s="11"/>
-      <c r="F182" s="20"/>
+      <c r="F182" s="25"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="21" t="s">
+      <c r="A183" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B183" s="21" t="s">
+      <c r="B183" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C183" s="5">
@@ -3516,13 +3516,13 @@
         <v>42</v>
       </c>
       <c r="E183" s="14"/>
-      <c r="F183" s="23" t="s">
+      <c r="F183" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="22"/>
-      <c r="B184" s="22"/>
+      <c r="A184" s="18"/>
+      <c r="B184" s="18"/>
       <c r="C184" s="5">
         <v>2</v>
       </c>
@@ -3530,11 +3530,11 @@
         <v>4</v>
       </c>
       <c r="E184" s="14"/>
-      <c r="F184" s="24"/>
+      <c r="F184" s="27"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="22"/>
-      <c r="B185" s="22"/>
+      <c r="A185" s="18"/>
+      <c r="B185" s="18"/>
       <c r="C185" s="5">
         <v>3</v>
       </c>
@@ -3542,11 +3542,11 @@
         <v>55</v>
       </c>
       <c r="E185" s="14"/>
-      <c r="F185" s="24"/>
+      <c r="F185" s="27"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="22"/>
-      <c r="B186" s="22"/>
+      <c r="A186" s="18"/>
+      <c r="B186" s="18"/>
       <c r="C186" s="5">
         <v>4</v>
       </c>
@@ -3554,11 +3554,11 @@
         <v>56</v>
       </c>
       <c r="E186" s="14"/>
-      <c r="F186" s="24"/>
+      <c r="F186" s="27"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="22"/>
-      <c r="B187" s="22"/>
+      <c r="A187" s="18"/>
+      <c r="B187" s="18"/>
       <c r="C187" s="5">
         <v>5</v>
       </c>
@@ -3566,11 +3566,11 @@
         <v>57</v>
       </c>
       <c r="E187" s="14"/>
-      <c r="F187" s="24"/>
+      <c r="F187" s="27"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="22"/>
-      <c r="B188" s="22"/>
+      <c r="A188" s="18"/>
+      <c r="B188" s="18"/>
       <c r="C188" s="5">
         <v>6</v>
       </c>
@@ -3578,13 +3578,13 @@
         <v>58</v>
       </c>
       <c r="E188" s="14"/>
-      <c r="F188" s="24"/>
+      <c r="F188" s="27"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="17" t="s">
+      <c r="A189" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B189" s="17" t="s">
+      <c r="B189" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C189" s="3">
@@ -3594,13 +3594,13 @@
         <v>42</v>
       </c>
       <c r="E189" s="11"/>
-      <c r="F189" s="19" t="s">
+      <c r="F189" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="18"/>
-      <c r="B190" s="18"/>
+      <c r="A190" s="21"/>
+      <c r="B190" s="21"/>
       <c r="C190" s="3">
         <v>2</v>
       </c>
@@ -3608,11 +3608,11 @@
         <v>4</v>
       </c>
       <c r="E190" s="11"/>
-      <c r="F190" s="20"/>
+      <c r="F190" s="25"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="18"/>
-      <c r="B191" s="18"/>
+      <c r="A191" s="21"/>
+      <c r="B191" s="21"/>
       <c r="C191" s="3">
         <v>3</v>
       </c>
@@ -3620,11 +3620,11 @@
         <v>55</v>
       </c>
       <c r="E191" s="11"/>
-      <c r="F191" s="20"/>
+      <c r="F191" s="25"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="18"/>
-      <c r="B192" s="18"/>
+      <c r="A192" s="21"/>
+      <c r="B192" s="21"/>
       <c r="C192" s="3">
         <v>4</v>
       </c>
@@ -3632,11 +3632,11 @@
         <v>56</v>
       </c>
       <c r="E192" s="11"/>
-      <c r="F192" s="20"/>
+      <c r="F192" s="25"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="18"/>
-      <c r="B193" s="18"/>
+      <c r="A193" s="21"/>
+      <c r="B193" s="21"/>
       <c r="C193" s="3">
         <v>5</v>
       </c>
@@ -3644,11 +3644,11 @@
         <v>57</v>
       </c>
       <c r="E193" s="11"/>
-      <c r="F193" s="20"/>
+      <c r="F193" s="25"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="18"/>
-      <c r="B194" s="18"/>
+      <c r="A194" s="21"/>
+      <c r="B194" s="21"/>
       <c r="C194" s="3">
         <v>6</v>
       </c>
@@ -3656,13 +3656,13 @@
         <v>58</v>
       </c>
       <c r="E194" s="11"/>
-      <c r="F194" s="20"/>
+      <c r="F194" s="25"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="21" t="s">
+      <c r="A195" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B195" s="21" t="s">
+      <c r="B195" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C195" s="5">
@@ -3672,13 +3672,13 @@
         <v>42</v>
       </c>
       <c r="E195" s="14"/>
-      <c r="F195" s="23" t="s">
+      <c r="F195" s="26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="22"/>
-      <c r="B196" s="22"/>
+      <c r="A196" s="18"/>
+      <c r="B196" s="18"/>
       <c r="C196" s="5">
         <v>2</v>
       </c>
@@ -3686,11 +3686,11 @@
         <v>4</v>
       </c>
       <c r="E196" s="14"/>
-      <c r="F196" s="24"/>
+      <c r="F196" s="27"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="22"/>
-      <c r="B197" s="22"/>
+      <c r="A197" s="18"/>
+      <c r="B197" s="18"/>
       <c r="C197" s="5">
         <v>3</v>
       </c>
@@ -3698,11 +3698,11 @@
         <v>55</v>
       </c>
       <c r="E197" s="14"/>
-      <c r="F197" s="24"/>
+      <c r="F197" s="27"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="22"/>
-      <c r="B198" s="22"/>
+      <c r="A198" s="18"/>
+      <c r="B198" s="18"/>
       <c r="C198" s="5">
         <v>4</v>
       </c>
@@ -3710,11 +3710,11 @@
         <v>56</v>
       </c>
       <c r="E198" s="14"/>
-      <c r="F198" s="24"/>
+      <c r="F198" s="27"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="22"/>
-      <c r="B199" s="22"/>
+      <c r="A199" s="18"/>
+      <c r="B199" s="18"/>
       <c r="C199" s="5">
         <v>5</v>
       </c>
@@ -3722,11 +3722,11 @@
         <v>57</v>
       </c>
       <c r="E199" s="14"/>
-      <c r="F199" s="24"/>
+      <c r="F199" s="27"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="22"/>
-      <c r="B200" s="22"/>
+      <c r="A200" s="18"/>
+      <c r="B200" s="18"/>
       <c r="C200" s="5">
         <v>6</v>
       </c>
@@ -3734,13 +3734,13 @@
         <v>58</v>
       </c>
       <c r="E200" s="14"/>
-      <c r="F200" s="24"/>
+      <c r="F200" s="27"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="17" t="s">
+      <c r="A201" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B201" s="17" t="s">
+      <c r="B201" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C201" s="3">
@@ -3750,13 +3750,13 @@
         <v>42</v>
       </c>
       <c r="E201" s="11"/>
-      <c r="F201" s="19" t="s">
+      <c r="F201" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="18"/>
-      <c r="B202" s="18"/>
+      <c r="A202" s="21"/>
+      <c r="B202" s="21"/>
       <c r="C202" s="3">
         <v>2</v>
       </c>
@@ -3764,11 +3764,11 @@
         <v>4</v>
       </c>
       <c r="E202" s="11"/>
-      <c r="F202" s="20"/>
+      <c r="F202" s="25"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="18"/>
-      <c r="B203" s="18"/>
+      <c r="A203" s="21"/>
+      <c r="B203" s="21"/>
       <c r="C203" s="3">
         <v>3</v>
       </c>
@@ -3776,11 +3776,11 @@
         <v>55</v>
       </c>
       <c r="E203" s="11"/>
-      <c r="F203" s="20"/>
+      <c r="F203" s="25"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="18"/>
-      <c r="B204" s="18"/>
+      <c r="A204" s="21"/>
+      <c r="B204" s="21"/>
       <c r="C204" s="3">
         <v>4</v>
       </c>
@@ -3788,11 +3788,11 @@
         <v>56</v>
       </c>
       <c r="E204" s="11"/>
-      <c r="F204" s="20"/>
+      <c r="F204" s="25"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="18"/>
-      <c r="B205" s="18"/>
+      <c r="A205" s="21"/>
+      <c r="B205" s="21"/>
       <c r="C205" s="3">
         <v>5</v>
       </c>
@@ -3800,11 +3800,11 @@
         <v>57</v>
       </c>
       <c r="E205" s="11"/>
-      <c r="F205" s="20"/>
+      <c r="F205" s="25"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="18"/>
-      <c r="B206" s="18"/>
+      <c r="A206" s="21"/>
+      <c r="B206" s="21"/>
       <c r="C206" s="3">
         <v>6</v>
       </c>
@@ -3812,13 +3812,13 @@
         <v>58</v>
       </c>
       <c r="E206" s="11"/>
-      <c r="F206" s="20"/>
+      <c r="F206" s="25"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="21" t="s">
+      <c r="A207" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B207" s="21" t="s">
+      <c r="B207" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C207" s="5">
@@ -3828,13 +3828,13 @@
         <v>42</v>
       </c>
       <c r="E207" s="14"/>
-      <c r="F207" s="23" t="s">
+      <c r="F207" s="26" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="22"/>
-      <c r="B208" s="22"/>
+      <c r="A208" s="18"/>
+      <c r="B208" s="18"/>
       <c r="C208" s="5">
         <v>2</v>
       </c>
@@ -3842,11 +3842,11 @@
         <v>4</v>
       </c>
       <c r="E208" s="14"/>
-      <c r="F208" s="24"/>
+      <c r="F208" s="27"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="22"/>
-      <c r="B209" s="22"/>
+      <c r="A209" s="18"/>
+      <c r="B209" s="18"/>
       <c r="C209" s="5">
         <v>3</v>
       </c>
@@ -3854,11 +3854,11 @@
         <v>55</v>
       </c>
       <c r="E209" s="14"/>
-      <c r="F209" s="24"/>
+      <c r="F209" s="27"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="22"/>
-      <c r="B210" s="22"/>
+      <c r="A210" s="18"/>
+      <c r="B210" s="18"/>
       <c r="C210" s="5">
         <v>4</v>
       </c>
@@ -3866,11 +3866,11 @@
         <v>56</v>
       </c>
       <c r="E210" s="14"/>
-      <c r="F210" s="24"/>
+      <c r="F210" s="27"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="22"/>
-      <c r="B211" s="22"/>
+      <c r="A211" s="18"/>
+      <c r="B211" s="18"/>
       <c r="C211" s="5">
         <v>5</v>
       </c>
@@ -3878,11 +3878,11 @@
         <v>57</v>
       </c>
       <c r="E211" s="14"/>
-      <c r="F211" s="24"/>
+      <c r="F211" s="27"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="22"/>
-      <c r="B212" s="22"/>
+      <c r="A212" s="18"/>
+      <c r="B212" s="18"/>
       <c r="C212" s="5">
         <v>6</v>
       </c>
@@ -3890,13 +3890,13 @@
         <v>58</v>
       </c>
       <c r="E212" s="14"/>
-      <c r="F212" s="24"/>
+      <c r="F212" s="27"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="17" t="s">
+      <c r="A213" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B213" s="17" t="s">
+      <c r="B213" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C213" s="3">
@@ -3906,13 +3906,13 @@
         <v>42</v>
       </c>
       <c r="E213" s="11"/>
-      <c r="F213" s="19" t="s">
+      <c r="F213" s="28" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="18"/>
-      <c r="B214" s="18"/>
+      <c r="A214" s="21"/>
+      <c r="B214" s="21"/>
       <c r="C214" s="3">
         <v>2</v>
       </c>
@@ -3920,11 +3920,11 @@
         <v>4</v>
       </c>
       <c r="E214" s="11"/>
-      <c r="F214" s="20"/>
+      <c r="F214" s="25"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="18"/>
-      <c r="B215" s="18"/>
+      <c r="A215" s="21"/>
+      <c r="B215" s="21"/>
       <c r="C215" s="3">
         <v>3</v>
       </c>
@@ -3932,11 +3932,11 @@
         <v>55</v>
       </c>
       <c r="E215" s="11"/>
-      <c r="F215" s="20"/>
+      <c r="F215" s="25"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="18"/>
-      <c r="B216" s="18"/>
+      <c r="A216" s="21"/>
+      <c r="B216" s="21"/>
       <c r="C216" s="3">
         <v>4</v>
       </c>
@@ -3944,11 +3944,11 @@
         <v>56</v>
       </c>
       <c r="E216" s="11"/>
-      <c r="F216" s="20"/>
+      <c r="F216" s="25"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="18"/>
-      <c r="B217" s="18"/>
+      <c r="A217" s="21"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="3">
         <v>5</v>
       </c>
@@ -3956,11 +3956,11 @@
         <v>57</v>
       </c>
       <c r="E217" s="11"/>
-      <c r="F217" s="20"/>
+      <c r="F217" s="25"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="18"/>
-      <c r="B218" s="18"/>
+      <c r="A218" s="21"/>
+      <c r="B218" s="21"/>
       <c r="C218" s="3">
         <v>6</v>
       </c>
@@ -3968,13 +3968,13 @@
         <v>58</v>
       </c>
       <c r="E218" s="11"/>
-      <c r="F218" s="20"/>
+      <c r="F218" s="25"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="21" t="s">
+      <c r="A219" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B219" s="21" t="s">
+      <c r="B219" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C219" s="5">
@@ -3984,13 +3984,13 @@
         <v>42</v>
       </c>
       <c r="E219" s="14"/>
-      <c r="F219" s="23" t="s">
+      <c r="F219" s="26" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="22"/>
-      <c r="B220" s="22"/>
+      <c r="A220" s="18"/>
+      <c r="B220" s="18"/>
       <c r="C220" s="5">
         <v>2</v>
       </c>
@@ -3998,11 +3998,11 @@
         <v>4</v>
       </c>
       <c r="E220" s="14"/>
-      <c r="F220" s="24"/>
+      <c r="F220" s="27"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="22"/>
-      <c r="B221" s="22"/>
+      <c r="A221" s="18"/>
+      <c r="B221" s="18"/>
       <c r="C221" s="5">
         <v>3</v>
       </c>
@@ -4010,11 +4010,11 @@
         <v>55</v>
       </c>
       <c r="E221" s="14"/>
-      <c r="F221" s="24"/>
+      <c r="F221" s="27"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="22"/>
-      <c r="B222" s="22"/>
+      <c r="A222" s="18"/>
+      <c r="B222" s="18"/>
       <c r="C222" s="5">
         <v>4</v>
       </c>
@@ -4022,11 +4022,11 @@
         <v>56</v>
       </c>
       <c r="E222" s="14"/>
-      <c r="F222" s="24"/>
+      <c r="F222" s="27"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="22"/>
-      <c r="B223" s="22"/>
+      <c r="A223" s="18"/>
+      <c r="B223" s="18"/>
       <c r="C223" s="5">
         <v>5</v>
       </c>
@@ -4034,11 +4034,11 @@
         <v>57</v>
       </c>
       <c r="E223" s="14"/>
-      <c r="F223" s="24"/>
+      <c r="F223" s="27"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="22"/>
-      <c r="B224" s="22"/>
+      <c r="A224" s="18"/>
+      <c r="B224" s="18"/>
       <c r="C224" s="5">
         <v>6</v>
       </c>
@@ -4046,13 +4046,13 @@
         <v>58</v>
       </c>
       <c r="E224" s="14"/>
-      <c r="F224" s="24"/>
+      <c r="F224" s="27"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="17" t="s">
+      <c r="A225" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B225" s="17" t="s">
+      <c r="B225" s="20" t="s">
         <v>53</v>
       </c>
       <c r="C225" s="3">
@@ -4062,13 +4062,13 @@
         <v>42</v>
       </c>
       <c r="E225" s="11"/>
-      <c r="F225" s="19" t="s">
+      <c r="F225" s="28" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="18"/>
-      <c r="B226" s="17"/>
+      <c r="A226" s="21"/>
+      <c r="B226" s="20"/>
       <c r="C226" s="3">
         <v>2</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>4</v>
       </c>
       <c r="E226" s="11"/>
-      <c r="F226" s="19"/>
+      <c r="F226" s="28"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C227"/>
@@ -4092,15 +4092,77 @@
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A97:A104"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="B106:B115"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="B97:B104"/>
-    <mergeCell ref="F97:F104"/>
+    <mergeCell ref="A225:A226"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="F225:F226"/>
+    <mergeCell ref="A213:A218"/>
+    <mergeCell ref="B213:B218"/>
+    <mergeCell ref="F213:F218"/>
+    <mergeCell ref="A219:A224"/>
+    <mergeCell ref="B219:B224"/>
+    <mergeCell ref="F219:F224"/>
+    <mergeCell ref="F207:F212"/>
+    <mergeCell ref="A189:A194"/>
+    <mergeCell ref="B189:B194"/>
+    <mergeCell ref="F189:F194"/>
+    <mergeCell ref="A195:A200"/>
+    <mergeCell ref="B195:B200"/>
+    <mergeCell ref="F195:F200"/>
+    <mergeCell ref="A201:A206"/>
+    <mergeCell ref="B201:B206"/>
+    <mergeCell ref="F201:F206"/>
+    <mergeCell ref="A207:A212"/>
+    <mergeCell ref="B207:B212"/>
+    <mergeCell ref="A177:A182"/>
+    <mergeCell ref="B177:B182"/>
+    <mergeCell ref="F177:F182"/>
+    <mergeCell ref="A183:A188"/>
+    <mergeCell ref="B183:B188"/>
+    <mergeCell ref="F183:F188"/>
+    <mergeCell ref="A166:A170"/>
+    <mergeCell ref="B166:B170"/>
+    <mergeCell ref="F166:F170"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="B171:B176"/>
+    <mergeCell ref="F171:F176"/>
+    <mergeCell ref="A156:A160"/>
+    <mergeCell ref="B156:B160"/>
+    <mergeCell ref="F156:F160"/>
+    <mergeCell ref="A161:A165"/>
+    <mergeCell ref="B161:B165"/>
+    <mergeCell ref="F161:F165"/>
+    <mergeCell ref="A145:F145"/>
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="F146:F150"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="B151:B155"/>
+    <mergeCell ref="F151:F155"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="B134:B138"/>
+    <mergeCell ref="F134:F138"/>
+    <mergeCell ref="A139:A144"/>
+    <mergeCell ref="B139:B144"/>
+    <mergeCell ref="F139:F144"/>
+    <mergeCell ref="A126:F126"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="F127:F128"/>
+    <mergeCell ref="F129:F133"/>
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="B129:B133"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="B89:B92"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A81:A88"/>
+    <mergeCell ref="B81:B88"/>
+    <mergeCell ref="A65:A72"/>
+    <mergeCell ref="B65:B72"/>
+    <mergeCell ref="A73:A80"/>
+    <mergeCell ref="B73:B80"/>
     <mergeCell ref="B116:B125"/>
     <mergeCell ref="A116:A125"/>
     <mergeCell ref="A2:F2"/>
@@ -4117,77 +4179,15 @@
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B18"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="B81:B88"/>
-    <mergeCell ref="A65:A72"/>
-    <mergeCell ref="B65:B72"/>
-    <mergeCell ref="A73:A80"/>
-    <mergeCell ref="B73:B80"/>
-    <mergeCell ref="A126:F126"/>
-    <mergeCell ref="B127:B128"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="F127:F128"/>
-    <mergeCell ref="F129:F133"/>
-    <mergeCell ref="A129:A133"/>
-    <mergeCell ref="B129:B133"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="B134:B138"/>
-    <mergeCell ref="F134:F138"/>
-    <mergeCell ref="A139:A144"/>
-    <mergeCell ref="B139:B144"/>
-    <mergeCell ref="F139:F144"/>
-    <mergeCell ref="A145:F145"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="F146:F150"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="B151:B155"/>
-    <mergeCell ref="F151:F155"/>
-    <mergeCell ref="A156:A160"/>
-    <mergeCell ref="B156:B160"/>
-    <mergeCell ref="F156:F160"/>
-    <mergeCell ref="A161:A165"/>
-    <mergeCell ref="B161:B165"/>
-    <mergeCell ref="F161:F165"/>
-    <mergeCell ref="A166:A170"/>
-    <mergeCell ref="B166:B170"/>
-    <mergeCell ref="F166:F170"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="B171:B176"/>
-    <mergeCell ref="F171:F176"/>
-    <mergeCell ref="A177:A182"/>
-    <mergeCell ref="B177:B182"/>
-    <mergeCell ref="F177:F182"/>
-    <mergeCell ref="A183:A188"/>
-    <mergeCell ref="B183:B188"/>
-    <mergeCell ref="F183:F188"/>
-    <mergeCell ref="F207:F212"/>
-    <mergeCell ref="A189:A194"/>
-    <mergeCell ref="B189:B194"/>
-    <mergeCell ref="F189:F194"/>
-    <mergeCell ref="A195:A200"/>
-    <mergeCell ref="B195:B200"/>
-    <mergeCell ref="F195:F200"/>
-    <mergeCell ref="A201:A206"/>
-    <mergeCell ref="B201:B206"/>
-    <mergeCell ref="F201:F206"/>
-    <mergeCell ref="A207:A212"/>
-    <mergeCell ref="B207:B212"/>
-    <mergeCell ref="A225:A226"/>
-    <mergeCell ref="B225:B226"/>
-    <mergeCell ref="F225:F226"/>
-    <mergeCell ref="A213:A218"/>
-    <mergeCell ref="B213:B218"/>
-    <mergeCell ref="F213:F218"/>
-    <mergeCell ref="A219:A224"/>
-    <mergeCell ref="B219:B224"/>
-    <mergeCell ref="F219:F224"/>
+    <mergeCell ref="A97:A104"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="B106:B115"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="A93:A96"/>
+    <mergeCell ref="B97:B104"/>
+    <mergeCell ref="F97:F104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>